<commit_message>
initial start, added TextMeshPro
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6DE5AE-091D-4F1E-97CE-F556A8C0B93C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C824354-F7AB-4A6A-8E5F-2DF0813DE754}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Key</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Welcome!</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Rock Quest</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +418,14 @@
         <v>50</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
some more magma chamber stuff, initial data for mineral/rock
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B635CA-2670-4B30-A1F5-2DC011BC6631}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EB8B0-C9C0-492B-938F-7D8EE5B75D8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Key</t>
   </si>
@@ -50,6 +50,69 @@
   </si>
   <si>
     <t>VICTORY</t>
+  </si>
+  <si>
+    <t>quartz</t>
+  </si>
+  <si>
+    <t>olivine</t>
+  </si>
+  <si>
+    <t>Olivine</t>
+  </si>
+  <si>
+    <t>olivineDesc</t>
+  </si>
+  <si>
+    <t>It's green.</t>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>quartzDesc</t>
+  </si>
+  <si>
+    <t>Colorful and crystally.</t>
+  </si>
+  <si>
+    <t>peridotite</t>
+  </si>
+  <si>
+    <t>Peridotite</t>
+  </si>
+  <si>
+    <t>peridotiteDesc</t>
+  </si>
+  <si>
+    <t>Igneous rock.</t>
+  </si>
+  <si>
+    <t>gabbro</t>
+  </si>
+  <si>
+    <t>Gabbro</t>
+  </si>
+  <si>
+    <t>gabbroDesc</t>
+  </si>
+  <si>
+    <t>diorite</t>
+  </si>
+  <si>
+    <t>Diorite</t>
+  </si>
+  <si>
+    <t>dioriteDesc</t>
+  </si>
+  <si>
+    <t>granite</t>
+  </si>
+  <si>
+    <t>Granite</t>
+  </si>
+  <si>
+    <t>graniteDesc</t>
   </si>
 </sst>
 </file>
@@ -382,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +506,138 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
more gameflow, start -> level 2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6EB8B0-C9C0-492B-938F-7D8EE5B75D8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E985334-5952-409B-BDB1-D2CE3B73D7D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Key</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>graniteDesc</t>
+  </si>
+  <si>
+    <t>igneous</t>
+  </si>
+  <si>
+    <t>sedimentary</t>
+  </si>
+  <si>
+    <t>metamorphic</t>
+  </si>
+  <si>
+    <t>Igneous</t>
+  </si>
+  <si>
+    <t>Sedimentary</t>
+  </si>
+  <si>
+    <t>Metamorphic</t>
   </si>
 </sst>
 </file>
@@ -445,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,133 +526,157 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>0.6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>0.6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="C19">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
offscreen goal display, setup placeholder extrusive rocks, setup sedimentary interaction
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E985334-5952-409B-BDB1-D2CE3B73D7D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47887454-A987-4558-9267-8169FB97E8A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Key</t>
   </si>
@@ -131,6 +131,45 @@
   </si>
   <si>
     <t>Metamorphic</t>
+  </si>
+  <si>
+    <t>pumice</t>
+  </si>
+  <si>
+    <t>Pumice</t>
+  </si>
+  <si>
+    <t>pumiceDesc</t>
+  </si>
+  <si>
+    <t>Igneous rock. Extrusive</t>
+  </si>
+  <si>
+    <t>scoria</t>
+  </si>
+  <si>
+    <t>Scoria</t>
+  </si>
+  <si>
+    <t>scoriaDesc</t>
+  </si>
+  <si>
+    <t>Rhyolite</t>
+  </si>
+  <si>
+    <t>rhyolite</t>
+  </si>
+  <si>
+    <t>rhyoliteDesc</t>
+  </si>
+  <si>
+    <t>basalt</t>
+  </si>
+  <si>
+    <t>Basalt</t>
+  </si>
+  <si>
+    <t>basaltDesc</t>
   </si>
 </sst>
 </file>
@@ -463,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +719,94 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
test out sedimentary processes, some fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47887454-A987-4558-9267-8169FB97E8A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE79525-F355-4E72-9567-5BCA857B2B04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Key</t>
   </si>
@@ -170,6 +170,126 @@
   </si>
   <si>
     <t>basaltDesc</t>
+  </si>
+  <si>
+    <t>breccia</t>
+  </si>
+  <si>
+    <t>Breccia</t>
+  </si>
+  <si>
+    <t>brecciaDesc</t>
+  </si>
+  <si>
+    <t>Sedimentary rock. Clastic</t>
+  </si>
+  <si>
+    <t>sandstone</t>
+  </si>
+  <si>
+    <t>Sandstone</t>
+  </si>
+  <si>
+    <t>sandstoneDesc</t>
+  </si>
+  <si>
+    <t>shale</t>
+  </si>
+  <si>
+    <t>Shale</t>
+  </si>
+  <si>
+    <t>shaleDesc</t>
+  </si>
+  <si>
+    <t>siltstone</t>
+  </si>
+  <si>
+    <t>Siltstone</t>
+  </si>
+  <si>
+    <t>siltstoneDesc</t>
+  </si>
+  <si>
+    <t>bituminousCoal</t>
+  </si>
+  <si>
+    <t>Bituminous Coal</t>
+  </si>
+  <si>
+    <t>bituminousCoalDesc</t>
+  </si>
+  <si>
+    <t>Sedimentary rock. Organic</t>
+  </si>
+  <si>
+    <t>limestone</t>
+  </si>
+  <si>
+    <t>Limestone</t>
+  </si>
+  <si>
+    <t>limestoneDesc</t>
+  </si>
+  <si>
+    <t>grainSize_LargeVariant</t>
+  </si>
+  <si>
+    <t>grainSize_Sand</t>
+  </si>
+  <si>
+    <t>grainSize_Silt</t>
+  </si>
+  <si>
+    <t>grainSize_Clay</t>
+  </si>
+  <si>
+    <t>grainSize_FineCourseCrystal</t>
+  </si>
+  <si>
+    <t>grainSize_Coarse</t>
+  </si>
+  <si>
+    <t>Pebbles, cobbles, and boulders.</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Fine to coarse crystals.</t>
+  </si>
+  <si>
+    <t>Microscopic to very coarse.</t>
+  </si>
+  <si>
+    <t>calcite</t>
+  </si>
+  <si>
+    <t>Calcite</t>
+  </si>
+  <si>
+    <t>calciteDesc</t>
+  </si>
+  <si>
+    <t>Shells, bones, etc.</t>
+  </si>
+  <si>
+    <t>carbon</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>carbonDesc</t>
+  </si>
+  <si>
+    <t>Dead plants and poop.</t>
   </si>
 </sst>
 </file>
@@ -502,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,76 +709,58 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>0.6</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
-        <v>0.6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>0.6</v>
@@ -666,10 +768,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -677,10 +779,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>0.6</v>
@@ -688,10 +790,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -699,10 +801,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="C18">
         <v>0.6</v>
@@ -710,10 +812,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -721,10 +823,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="C20">
         <v>0.6</v>
@@ -732,10 +834,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -743,21 +845,21 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -765,10 +867,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>0.6</v>
@@ -776,10 +878,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -787,10 +889,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>0.6</v>
@@ -798,12 +900,254 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C27">
+      <c r="C37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjustments to rock data, added initial metamorphic rock data, change sedimentary clastic to require 3 types of rocks.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE79525-F355-4E72-9567-5BCA857B2B04}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7987ECBA-68EA-4CC5-8722-F9E9851F090E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
   <si>
     <t>Key</t>
   </si>
@@ -290,6 +290,15 @@
   </si>
   <si>
     <t>Dead plants and poop.</t>
+  </si>
+  <si>
+    <t>obsidian</t>
+  </si>
+  <si>
+    <t>Obsidian</t>
+  </si>
+  <si>
+    <t>obsidianDesc</t>
   </si>
 </sst>
 </file>
@@ -622,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,21 +1030,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="C38">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -1043,10 +1052,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C40">
         <v>0.6</v>
@@ -1054,7 +1063,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
         <v>53</v>
@@ -1065,10 +1074,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C42">
         <v>0.6</v>
@@ -1076,7 +1085,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B43" t="s">
         <v>53</v>
@@ -1087,10 +1096,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C44">
         <v>0.6</v>
@@ -1098,7 +1107,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
         <v>53</v>
@@ -1109,21 +1118,21 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -1131,23 +1140,45 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
       </c>
       <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
interface bug fixes, reduce total levels to 5, testing gameflow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7987ECBA-68EA-4CC5-8722-F9E9851F090E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276408EB-70BB-4FFA-8FC0-B17B09F6F2E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
   <si>
     <t>Key</t>
   </si>
@@ -299,6 +299,90 @@
   </si>
   <si>
     <t>obsidianDesc</t>
+  </si>
+  <si>
+    <t>amphibolite</t>
+  </si>
+  <si>
+    <t>Amphibolite</t>
+  </si>
+  <si>
+    <t>amphiboliteDesc</t>
+  </si>
+  <si>
+    <t>Metamorphic rock.</t>
+  </si>
+  <si>
+    <t>anthraciteCoal</t>
+  </si>
+  <si>
+    <t>Anthracite Coal</t>
+  </si>
+  <si>
+    <t>anthraciteCoalDesc</t>
+  </si>
+  <si>
+    <t>gneiss</t>
+  </si>
+  <si>
+    <t>Gneiss</t>
+  </si>
+  <si>
+    <t>gneissDesc</t>
+  </si>
+  <si>
+    <t>marble</t>
+  </si>
+  <si>
+    <t>Marble</t>
+  </si>
+  <si>
+    <t>marbleDesc</t>
+  </si>
+  <si>
+    <t>metaconglomerate</t>
+  </si>
+  <si>
+    <t>Metaconglomerate</t>
+  </si>
+  <si>
+    <t>metaconglomerateDesc</t>
+  </si>
+  <si>
+    <t>phyllite</t>
+  </si>
+  <si>
+    <t>Phyllite</t>
+  </si>
+  <si>
+    <t>phylliteDesc</t>
+  </si>
+  <si>
+    <t>quartzite</t>
+  </si>
+  <si>
+    <t>Quartzite</t>
+  </si>
+  <si>
+    <t>quartziteDesc</t>
+  </si>
+  <si>
+    <t>schist</t>
+  </si>
+  <si>
+    <t>Schist</t>
+  </si>
+  <si>
+    <t>schistDesc</t>
+  </si>
+  <si>
+    <t>slate</t>
+  </si>
+  <si>
+    <t>Slate</t>
+  </si>
+  <si>
+    <t>slateDesc</t>
   </si>
 </sst>
 </file>
@@ -631,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,6 +1266,204 @@
         <v>5</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>93</v>
+      </c>
+      <c r="B52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
more level 1 stuff, initial setup of the other minerals
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276408EB-70BB-4FFA-8FC0-B17B09F6F2E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB86E1-F32F-4C97-B833-FE0292F6B2DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
   <si>
     <t>Key</t>
   </si>
@@ -64,18 +64,12 @@
     <t>olivineDesc</t>
   </si>
   <si>
-    <t>It's green.</t>
-  </si>
-  <si>
     <t>Quartz</t>
   </si>
   <si>
     <t>quartzDesc</t>
   </si>
   <si>
-    <t>Colorful and crystally.</t>
-  </si>
-  <si>
     <t>peridotite</t>
   </si>
   <si>
@@ -383,6 +377,45 @@
   </si>
   <si>
     <t>slateDesc</t>
+  </si>
+  <si>
+    <t>mineral</t>
+  </si>
+  <si>
+    <t>feldspar</t>
+  </si>
+  <si>
+    <t>Feldspar</t>
+  </si>
+  <si>
+    <t>feldsparDesc</t>
+  </si>
+  <si>
+    <t>pyroxene</t>
+  </si>
+  <si>
+    <t>Pyroxene</t>
+  </si>
+  <si>
+    <t>pyroxeneDesc</t>
+  </si>
+  <si>
+    <t>amphibole</t>
+  </si>
+  <si>
+    <t>Amphibole</t>
+  </si>
+  <si>
+    <t>amphiboleDesc</t>
+  </si>
+  <si>
+    <t>biotite</t>
+  </si>
+  <si>
+    <t>Biotite</t>
+  </si>
+  <si>
+    <t>biotiteDesc</t>
   </si>
 </sst>
 </file>
@@ -715,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,74 +811,74 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,7 +897,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -875,7 +908,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>0.6</v>
@@ -883,10 +916,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -894,21 +927,21 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="C18">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -916,21 +949,21 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C20">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C21">
         <v>5</v>
@@ -938,10 +971,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -949,10 +982,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -960,10 +993,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="C24">
         <v>0.6</v>
@@ -971,10 +1004,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="C25">
         <v>5</v>
@@ -982,10 +1015,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <v>0.6</v>
@@ -993,10 +1026,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -1004,10 +1037,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C28">
         <v>0.6</v>
@@ -1015,10 +1048,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -1026,21 +1059,21 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -1048,10 +1081,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <v>0.6</v>
@@ -1059,10 +1092,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -1070,10 +1103,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C34">
         <v>0.6</v>
@@ -1081,10 +1114,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -1092,10 +1125,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C36">
         <v>0.6</v>
@@ -1103,10 +1136,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -1114,21 +1147,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -1136,10 +1169,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>0.6</v>
@@ -1147,10 +1180,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -1158,10 +1191,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C42">
         <v>0.6</v>
@@ -1169,10 +1202,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C43">
         <v>5</v>
@@ -1180,10 +1213,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>0.6</v>
@@ -1191,10 +1224,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1202,21 +1235,21 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C46">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -1224,21 +1257,21 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -1246,21 +1279,21 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C50">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -1268,21 +1301,21 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -1290,21 +1323,21 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -1312,21 +1345,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="C56">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -1334,21 +1367,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="C58">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C59">
         <v>5</v>
@@ -1356,21 +1389,21 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C60">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C61">
         <v>5</v>
@@ -1378,21 +1411,21 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C62">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -1400,21 +1433,21 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B64" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C65">
         <v>5</v>
@@ -1422,21 +1455,21 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C66">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C67">
         <v>5</v>
@@ -1444,23 +1477,111 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C68">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>107</v>
+      </c>
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>109</v>
+      </c>
+      <c r="B71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" t="s">
+        <v>114</v>
+      </c>
+      <c r="C74">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" t="s">
+        <v>94</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated modules, plugins; added UIExt, Shape2D; removed TextMesh Pro stuff; some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB86E1-F32F-4C97-B833-FE0292F6B2DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4371C570-F9D5-4C32-B57C-C47C2D6E11E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3225" yWindow="2415" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
   <si>
     <t>Key</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>biotiteDesc</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>* NEW *</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,753 +841,761 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>0.6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C16">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C24">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C26">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C28">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C38">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C42">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C44">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C48">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C52">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C54">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C58">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C64">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C66">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C68">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C70">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C74">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C76">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" t="s">
+        <v>117</v>
+      </c>
+      <c r="C77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>118</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>94</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
various ui art update in magma chamber, changed gameflow to suit animations
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4371C570-F9D5-4C32-B57C-C47C2D6E11E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1406FCD-E7CF-4CD5-BAE6-721114C1120B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="2415" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
   <si>
     <t>Key</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t>* NEW *</t>
+  </si>
+  <si>
+    <t>magma_title</t>
+  </si>
+  <si>
+    <t>MAGMA</t>
   </si>
 </sst>
 </file>
@@ -754,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,753 +855,761 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15">
-        <v>0.6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C17">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C25">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C27">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C37">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C39">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C43">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C45">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C49">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C53">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C55">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C59">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B64" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C65">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C67">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C69">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C71">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B74" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B75" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C75">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B77" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C77">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>116</v>
+      </c>
+      <c r="B78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C78">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>118</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>94</v>
       </c>
-      <c r="C78">
+      <c r="C79">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial magma chamber doodad draft
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1406FCD-E7CF-4CD5-BAE6-721114C1120B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ADECCA-51BA-49CF-872C-717D235CAD54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3225" yWindow="2415" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="138">
   <si>
     <t>Key</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>MAGMA</t>
+  </si>
+  <si>
+    <t>minerals</t>
+  </si>
+  <si>
+    <t>Minerals</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,753 +869,761 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
-        <v>0.6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C18">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C26">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C28">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C34">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C36">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C38">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C42">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C44">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C46">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C50">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C52">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C54">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C56">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C60">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C66">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C68">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C70">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C72">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B73" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B74" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C76">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C78">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>116</v>
+      </c>
+      <c r="B79" t="s">
+        <v>117</v>
+      </c>
+      <c r="C79">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>118</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>94</v>
       </c>
-      <c r="C79">
+      <c r="C80">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some ui art for magmaCooler scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD4863B-82BB-438B-A5D7-59B286F7DE67}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3203B141-5F2F-442E-840D-ECE8C5C027F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="2415" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
   <si>
     <t>Key</t>
   </si>
@@ -500,6 +500,48 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>select_method</t>
+  </si>
+  <si>
+    <t>Select Method</t>
+  </si>
+  <si>
+    <t>intrusive</t>
+  </si>
+  <si>
+    <t>Intrusive</t>
+  </si>
+  <si>
+    <t>extrusive</t>
+  </si>
+  <si>
+    <t>Extrusive</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>BACK</t>
+  </si>
+  <si>
+    <t>proceed</t>
+  </si>
+  <si>
+    <t>PROCEED</t>
+  </si>
+  <si>
+    <t>cooling</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>Cooling…</t>
   </si>
 </sst>
 </file>
@@ -832,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,812 +1014,868 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28">
-        <v>0.6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
-        <v>0.6</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C38">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C40">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C42">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="C46">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C48">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="C50">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C52">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C56">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C58">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C62">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C64">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C66">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C68">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C72">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C78">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C80">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C82">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C84">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C88">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C90">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>107</v>
+      </c>
+      <c r="B91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" t="s">
+        <v>111</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>112</v>
+      </c>
+      <c r="B94" t="s">
+        <v>94</v>
+      </c>
+      <c r="C94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" t="s">
+        <v>114</v>
+      </c>
+      <c r="C95">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B97" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>118</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B98" t="s">
         <v>94</v>
       </c>
-      <c r="C91">
+      <c r="C98">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more ui refurbish in magmaCooler scene
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3203B141-5F2F-442E-840D-ECE8C5C027F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54259C66-917B-42C5-92C4-A7E11B6B3B5A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="178">
   <si>
     <t>Key</t>
   </si>
@@ -542,6 +542,18 @@
   </si>
   <si>
     <t>Cooling…</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>rock_result</t>
+  </si>
+  <si>
+    <t>ROCK RESULT</t>
   </si>
 </sst>
 </file>
@@ -874,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,80 +1141,74 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>176</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35">
-        <v>0.6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36">
-        <v>5</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C37">
         <v>0.6</v>
@@ -1210,7 +1216,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
         <v>119</v>
@@ -1221,18 +1227,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
         <v>119</v>
@@ -1243,10 +1249,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1254,7 +1260,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
         <v>119</v>
@@ -1265,10 +1271,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1276,7 +1282,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
         <v>119</v>
@@ -1287,18 +1293,18 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C45">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
         <v>119</v>
@@ -1309,10 +1315,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="C47">
         <v>0.6</v>
@@ -1320,10 +1326,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="C48">
         <v>5</v>
@@ -1331,10 +1337,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C49">
         <v>0.6</v>
@@ -1342,10 +1348,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C50">
         <v>5</v>
@@ -1353,21 +1359,21 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="C52">
         <v>5</v>
@@ -1375,18 +1381,18 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
@@ -1397,10 +1403,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C55">
         <v>0.6</v>
@@ -1408,7 +1414,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
@@ -1419,10 +1425,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C57">
         <v>0.6</v>
@@ -1430,7 +1436,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
@@ -1441,10 +1447,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C59">
         <v>0.6</v>
@@ -1452,10 +1458,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>5</v>
@@ -1463,10 +1469,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C61">
         <v>0.6</v>
@@ -1474,7 +1480,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B62" t="s">
         <v>38</v>
@@ -1485,10 +1491,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C63">
         <v>0.6</v>
@@ -1496,7 +1502,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B64" t="s">
         <v>38</v>
@@ -1507,10 +1513,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C65">
         <v>0.6</v>
@@ -1518,7 +1524,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B66" t="s">
         <v>38</v>
@@ -1529,18 +1535,18 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
         <v>38</v>
@@ -1551,21 +1557,21 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="C69">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C70">
         <v>5</v>
@@ -1573,10 +1579,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C71">
         <v>0.6</v>
@@ -1584,7 +1590,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B72" t="s">
         <v>51</v>
@@ -1595,10 +1601,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C73">
         <v>0.6</v>
@@ -1606,7 +1612,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B74" t="s">
         <v>51</v>
@@ -1617,10 +1623,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C75">
         <v>0.6</v>
@@ -1628,7 +1634,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
         <v>51</v>
@@ -1639,21 +1645,21 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B77" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C78">
         <v>5</v>
@@ -1661,18 +1667,18 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C79">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B80" t="s">
         <v>64</v>
@@ -1683,21 +1689,21 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B81" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="C82">
         <v>5</v>
@@ -1705,18 +1711,18 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
         <v>94</v>
@@ -1727,18 +1733,18 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C85">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -1749,18 +1755,18 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C87">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
         <v>94</v>
@@ -1771,18 +1777,18 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B89" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C89">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B90" t="s">
         <v>94</v>
@@ -1793,18 +1799,18 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C91">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B92" t="s">
         <v>94</v>
@@ -1815,18 +1821,18 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B93" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
         <v>94</v>
@@ -1837,18 +1843,18 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B95" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C95">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B96" t="s">
         <v>94</v>
@@ -1859,10 +1865,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B97" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C97">
         <v>0.5</v>
@@ -1870,12 +1876,34 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
         <v>94</v>
       </c>
       <c r="C98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>116</v>
+      </c>
+      <c r="B99" t="s">
+        <v>117</v>
+      </c>
+      <c r="C99">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
igneous rock textures redone, initial SedimentaryController reskin
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54259C66-917B-42C5-92C4-A7E11B6B3B5A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A709A41-B077-4666-8278-3761487BE930}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="184">
   <si>
     <t>Key</t>
   </si>
@@ -554,6 +554,24 @@
   </si>
   <si>
     <t>ROCK RESULT</t>
+  </si>
+  <si>
+    <t>select_source</t>
+  </si>
+  <si>
+    <t>Select Source</t>
+  </si>
+  <si>
+    <t>rocks</t>
+  </si>
+  <si>
+    <t>Rocks</t>
+  </si>
+  <si>
+    <t>organics</t>
+  </si>
+  <si>
+    <t>Organics</t>
   </si>
 </sst>
 </file>
@@ -886,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,876 +1052,900 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37">
-        <v>0.6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
-      </c>
-      <c r="C38">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39">
-        <v>0.6</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>14</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B45" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C47">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="C49">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C51">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C52">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B54" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C55">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C57">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C61">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C62">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C63">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C64">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C65">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C67">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C70">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C71">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C73">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C75">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C76">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B77" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C77">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C81">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B84" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B85" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C87">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C89">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C91">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C93">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B96" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C97">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C98">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B99" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="C99">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" t="s">
+        <v>114</v>
+      </c>
+      <c r="C100">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>115</v>
+      </c>
+      <c r="B101" t="s">
+        <v>94</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>116</v>
+      </c>
+      <c r="B102" t="s">
+        <v>117</v>
+      </c>
+      <c r="C102">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>118</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B103" t="s">
         <v>94</v>
       </c>
-      <c r="C100">
+      <c r="C103">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
redo sedimentary setup, near complete
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A709A41-B077-4666-8278-3761487BE930}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD604F88-A5BF-449C-8385-265E9869B397}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="188">
   <si>
     <t>Key</t>
   </si>
@@ -244,9 +244,6 @@
     <t>grainSize_Coarse</t>
   </si>
   <si>
-    <t>Pebbles, cobbles, and boulders.</t>
-  </si>
-  <si>
     <t>Sand</t>
   </si>
   <si>
@@ -572,6 +569,21 @@
   </si>
   <si>
     <t>Organics</t>
+  </si>
+  <si>
+    <t>erode</t>
+  </si>
+  <si>
+    <t>ERODE</t>
+  </si>
+  <si>
+    <t>grainSize</t>
+  </si>
+  <si>
+    <t>Cobbles</t>
+  </si>
+  <si>
+    <t>Grain Size</t>
   </si>
 </sst>
 </file>
@@ -904,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,154 +968,154 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
         <v>138</v>
-      </c>
-      <c r="B4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
         <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" t="s">
         <v>142</v>
-      </c>
-      <c r="B6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
         <v>144</v>
-      </c>
-      <c r="B7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" t="s">
         <v>146</v>
-      </c>
-      <c r="B8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="s">
         <v>149</v>
-      </c>
-      <c r="B9" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" t="s">
         <v>152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
         <v>154</v>
-      </c>
-      <c r="B12" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
         <v>156</v>
-      </c>
-      <c r="B13" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
         <v>158</v>
-      </c>
-      <c r="B14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
         <v>160</v>
-      </c>
-      <c r="B15" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" t="s">
         <v>178</v>
-      </c>
-      <c r="B16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
         <v>162</v>
-      </c>
-      <c r="B17" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
         <v>164</v>
-      </c>
-      <c r="B18" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" t="s">
         <v>180</v>
-      </c>
-      <c r="B19" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" t="s">
         <v>182</v>
-      </c>
-      <c r="B20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" t="s">
         <v>166</v>
-      </c>
-      <c r="B21" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" t="s">
         <v>168</v>
-      </c>
-      <c r="B22" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1143,136 +1155,130 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" t="s">
         <v>132</v>
-      </c>
-      <c r="B27" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" t="s">
         <v>134</v>
-      </c>
-      <c r="B28" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
         <v>136</v>
-      </c>
-      <c r="B29" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" t="s">
         <v>171</v>
-      </c>
-      <c r="B31" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" t="s">
         <v>176</v>
-      </c>
-      <c r="B32" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" t="s">
         <v>174</v>
-      </c>
-      <c r="B33" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>185</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40">
-        <v>0.6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C42">
         <v>0.6</v>
@@ -1280,10 +1286,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43">
         <v>5</v>
@@ -1291,21 +1297,21 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1313,10 +1319,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1324,10 +1330,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -1335,10 +1341,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B48" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1346,10 +1352,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -1357,21 +1363,21 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C50">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -1379,10 +1385,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="C52">
         <v>0.6</v>
@@ -1390,10 +1396,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -1401,10 +1407,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C54">
         <v>0.6</v>
@@ -1412,10 +1418,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C55">
         <v>5</v>
@@ -1423,21 +1429,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -1445,18 +1451,18 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C58">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
@@ -1467,10 +1473,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C60">
         <v>0.6</v>
@@ -1478,7 +1484,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
@@ -1489,10 +1495,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C62">
         <v>0.6</v>
@@ -1500,7 +1506,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
@@ -1511,10 +1517,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>0.6</v>
@@ -1522,10 +1528,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C65">
         <v>5</v>
@@ -1533,10 +1539,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C66">
         <v>0.6</v>
@@ -1544,7 +1550,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B67" t="s">
         <v>38</v>
@@ -1555,10 +1561,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C68">
         <v>0.6</v>
@@ -1566,7 +1572,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B69" t="s">
         <v>38</v>
@@ -1577,10 +1583,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C70">
         <v>0.6</v>
@@ -1588,7 +1594,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B71" t="s">
         <v>38</v>
@@ -1599,18 +1605,18 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B73" t="s">
         <v>38</v>
@@ -1621,21 +1627,21 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="C74">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C75">
         <v>5</v>
@@ -1643,10 +1649,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C76">
         <v>0.6</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B77" t="s">
         <v>51</v>
@@ -1665,10 +1671,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C78">
         <v>0.6</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B79" t="s">
         <v>51</v>
@@ -1687,10 +1693,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B80" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C80">
         <v>0.6</v>
@@ -1698,7 +1704,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B81" t="s">
         <v>51</v>
@@ -1709,21 +1715,21 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B82" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B83" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C83">
         <v>5</v>
@@ -1731,18 +1737,18 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C84">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B85" t="s">
         <v>64</v>
@@ -1753,21 +1759,21 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="C87">
         <v>5</v>
@@ -1775,21 +1781,21 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C89">
         <v>5</v>
@@ -1797,21 +1803,21 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C90">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C91">
         <v>5</v>
@@ -1819,21 +1825,21 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C92">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -1841,21 +1847,21 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C94">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C95">
         <v>5</v>
@@ -1863,21 +1869,21 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C96">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97">
         <v>5</v>
@@ -1885,21 +1891,21 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C99">
         <v>5</v>
@@ -1907,21 +1913,21 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C100">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B101" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C101">
         <v>5</v>
@@ -1929,10 +1935,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B102" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C102">
         <v>0.5</v>
@@ -1940,12 +1946,34 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>115</v>
+      </c>
+      <c r="B104" t="s">
+        <v>116</v>
+      </c>
+      <c r="C104">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" t="s">
+        <v>93</v>
+      </c>
+      <c r="C105">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modal info for rocks/minerals art update
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD604F88-A5BF-449C-8385-265E9869B397}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42FC7EE-0212-4739-8476-D6B54E3AB378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="190">
   <si>
     <t>Key</t>
   </si>
@@ -584,6 +584,12 @@
   </si>
   <si>
     <t>Grain Size</t>
+  </si>
+  <si>
+    <t>collections</t>
+  </si>
+  <si>
+    <t>COLLECTIONS</t>
   </si>
 </sst>
 </file>
@@ -916,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,849 +1137,860 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>189</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B32" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B35" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42">
-        <v>0.6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="C44">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C52">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C54">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C55">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C56">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C59">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C60">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C62">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C64">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B66" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C66">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C67">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C68">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C70">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C72">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C73">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="B74" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C76">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C77">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C78">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B79" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B80" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C80">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B82" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C82">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B83" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B84" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C86">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C92">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C93">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C94">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C95">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C96">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C98">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C99">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B100" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B101" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C101">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B102" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C102">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B103" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C103">
-        <v>5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="C104">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>115</v>
+      </c>
+      <c r="B105" t="s">
+        <v>116</v>
+      </c>
+      <c r="C105">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>117</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>93</v>
       </c>
-      <c r="C105">
+      <c r="C106">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
camera for background parallax, collection modal
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6E75A8-B8F1-4A8A-BD90-E5317B766D74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B1A016-C5B5-4BCA-9595-C188742E409A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="1785" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
level 1 and rock process dialogs
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC708ACD-0F51-4220-BCD1-E26B90E71D02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D0F6E6-7CF6-404A-98C7-C2B84A2BF881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3375" yWindow="1830" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1725" yWindow="1740" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="262">
   <si>
     <t>Key</t>
   </si>
@@ -616,9 +616,6 @@
     <t>Welcome to Super Gnomatic Rock Cycler!</t>
   </si>
   <si>
-    <t>We’ll be learning about the various processes of forming rocks.</t>
-  </si>
-  <si>
     <t>intro_2</t>
   </si>
   <si>
@@ -643,9 +640,6 @@
     <t>Rock</t>
   </si>
   <si>
-    <t>For now, let’s go ahead and gather some minerals!</t>
-  </si>
-  <si>
     <t>Press the Left or Right arrow key to move the Gnome.</t>
   </si>
   <si>
@@ -661,13 +655,157 @@
     <t>Depending on the minerals and how it was formed, a rock can have distinct characteristics.</t>
   </si>
   <si>
-    <t>We’ll look into more details on the different types of rocks later.</t>
-  </si>
-  <si>
     <t>instruction_jump</t>
   </si>
   <si>
     <t>Press the Spacebar or Up arrow to jump.</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_1</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_2</t>
+  </si>
+  <si>
+    <t>Head over to the Magma Chamber to do so.</t>
+  </si>
+  <si>
+    <t>magma_chamber</t>
+  </si>
+  <si>
+    <t>Magma Chamber</t>
+  </si>
+  <si>
+    <t>magma_cooler</t>
+  </si>
+  <si>
+    <t>Magma Cooler</t>
+  </si>
+  <si>
+    <t>Crust</t>
+  </si>
+  <si>
+    <t>mantle</t>
+  </si>
+  <si>
+    <t>Mantle</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>crust</t>
+  </si>
+  <si>
+    <t>intro_magma_chamber_1</t>
+  </si>
+  <si>
+    <t>intro_magma_chamber_2</t>
+  </si>
+  <si>
+    <t>intro_magma_chamber_3</t>
+  </si>
+  <si>
+    <t>intro_magma_chamber_4</t>
+  </si>
+  <si>
+    <t>On Earth, rocks are continuously pushed upward or downward due to physical activities such as an earthquake.</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_cooler_1</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_cooler_2</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_cooler_3</t>
+  </si>
+  <si>
+    <t>If you notice at the very top, we need to form at least three different types of igneous rock.</t>
+  </si>
+  <si>
+    <t>In order to form igneous rocks, head over to the Magma Cooler.</t>
+  </si>
+  <si>
+    <t>magma_require</t>
+  </si>
+  <si>
+    <t>We require magma to form igneous rocks. Head over to the Magma Chamber.</t>
+  </si>
+  <si>
+    <t>Go ahead and process the minerals by holding the Spacebar (you can also click and hold the icon).</t>
+  </si>
+  <si>
+    <t>intro_intrusive_igneous_1</t>
+  </si>
+  <si>
+    <t>intro_intrusive_igneous_2</t>
+  </si>
+  <si>
+    <t>intro_intrusive_igneous_3</t>
+  </si>
+  <si>
+    <t>intro_intrusive_igneous_4</t>
+  </si>
+  <si>
+    <t>intrusive_igneous_instruction</t>
+  </si>
+  <si>
+    <t>There are two ways for igneous rocks to form: intrusive or extrusive.</t>
+  </si>
+  <si>
+    <t>For now, we will form intrusive igneous rocks.</t>
+  </si>
+  <si>
+    <t>Intrusive rocks are formed when magma cools off below the Earth’s surface.</t>
+  </si>
+  <si>
+    <t>Press the Spacebar (or click STOP) to end the cooling process.</t>
+  </si>
+  <si>
+    <t>Remember to form at least three types of igneous rocks as indicated at the top.</t>
+  </si>
+  <si>
+    <t>submit_instruction_1</t>
+  </si>
+  <si>
+    <t>Now that you have formed the necessary rocks, it’s time to drop them off.</t>
+  </si>
+  <si>
+    <t>submit_instruction_2</t>
+  </si>
+  <si>
+    <t>Head over to the indicated star and submit the rocks!</t>
+  </si>
+  <si>
+    <t>Rocks pushed deep into the mantle's hot spots will melt to magma.</t>
+  </si>
+  <si>
+    <t>Now that we have magma available, it's time to form some rocks!</t>
+  </si>
+  <si>
+    <t>Now that you have some minerals, it's time to melt them down into magma.</t>
+  </si>
+  <si>
+    <t>We'll look into more details on the different types of rocks later.</t>
+  </si>
+  <si>
+    <t>We'll be learning about the various processes of forming rocks.</t>
+  </si>
+  <si>
+    <t>For now, let's go ahead and gather some minerals!</t>
+  </si>
+  <si>
+    <t>Here in the Magma Chamber, we can simulate the process of melting rocks to magma.</t>
+  </si>
+  <si>
+    <t>next_adventure_dialog_1</t>
+  </si>
+  <si>
+    <t>Excellent work! Now that the rocks have been submitted, we can gather more minerals to form new rocks.</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,10 +1337,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" t="s">
         <v>205</v>
-      </c>
-      <c r="B22" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1413,769 +1551,953 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>199</v>
       </c>
-      <c r="B48" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>201</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>204</v>
-      </c>
-      <c r="B53" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>209</v>
-      </c>
-      <c r="B54" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B56" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>214</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>227</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>228</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>121</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" t="s">
-        <v>117</v>
-      </c>
-      <c r="C63">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>233</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>126</v>
-      </c>
-      <c r="B65" t="s">
-        <v>117</v>
-      </c>
-      <c r="C65">
-        <v>5</v>
+        <v>239</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>127</v>
-      </c>
-      <c r="B66" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66">
-        <v>0.6</v>
+        <v>240</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>241</v>
       </c>
       <c r="B67" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67">
-        <v>5</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
-      </c>
-      <c r="B68" t="s">
-        <v>79</v>
-      </c>
-      <c r="C68">
-        <v>0.6</v>
+        <v>242</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69">
-        <v>5</v>
+        <v>243</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70">
-        <v>0.6</v>
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>251</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
-      </c>
-      <c r="C71">
-        <v>5</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>260</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
-      </c>
-      <c r="C73">
-        <v>5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>218</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74">
-        <v>0.6</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>21</v>
+        <v>236</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
-      </c>
-      <c r="C75">
-        <v>5</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76">
-        <v>0.6</v>
+        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>221</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
-      </c>
-      <c r="C77">
-        <v>5</v>
+        <v>222</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78">
-        <v>0.6</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C79">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B80" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="C80">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="C82">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="C84">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="B86" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C86">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="C90">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B92" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="C92">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B93" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="C93">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B94" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C94">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="B95" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C95">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C96">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="C99">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="B100" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C100">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C101">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B103" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="C103">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="B104" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C105">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="C106">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="C107">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="B108" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="C108">
-        <v>0.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C109">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
       <c r="C110">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B111" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C111">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="C112">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="B113" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="C113">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>108</v>
+        <v>49</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="B115" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="C115">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B116" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="C116">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="B117" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="C117">
-        <v>5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>115</v>
+        <v>50</v>
       </c>
       <c r="C118">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>57</v>
+      </c>
+      <c r="B119" t="s">
+        <v>58</v>
+      </c>
+      <c r="C119">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>59</v>
+      </c>
+      <c r="B120" t="s">
+        <v>50</v>
+      </c>
+      <c r="C120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>60</v>
+      </c>
+      <c r="B121" t="s">
+        <v>61</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>62</v>
+      </c>
+      <c r="B122" t="s">
+        <v>63</v>
+      </c>
+      <c r="C122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>64</v>
+      </c>
+      <c r="B123" t="s">
+        <v>65</v>
+      </c>
+      <c r="C123">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>66</v>
+      </c>
+      <c r="B124" t="s">
+        <v>63</v>
+      </c>
+      <c r="C124">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>89</v>
+      </c>
+      <c r="B125" t="s">
+        <v>90</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>91</v>
+      </c>
+      <c r="B126" t="s">
+        <v>92</v>
+      </c>
+      <c r="C126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>93</v>
+      </c>
+      <c r="B127" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>95</v>
+      </c>
+      <c r="B128" t="s">
+        <v>92</v>
+      </c>
+      <c r="C128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>96</v>
+      </c>
+      <c r="B129" t="s">
+        <v>97</v>
+      </c>
+      <c r="C129">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>98</v>
+      </c>
+      <c r="B130" t="s">
+        <v>92</v>
+      </c>
+      <c r="C130">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>99</v>
+      </c>
+      <c r="B131" t="s">
+        <v>100</v>
+      </c>
+      <c r="C131">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>101</v>
+      </c>
+      <c r="B132" t="s">
+        <v>92</v>
+      </c>
+      <c r="C132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>102</v>
+      </c>
+      <c r="B133" t="s">
+        <v>103</v>
+      </c>
+      <c r="C133">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>104</v>
+      </c>
+      <c r="B134" t="s">
+        <v>92</v>
+      </c>
+      <c r="C134">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>105</v>
+      </c>
+      <c r="B135" t="s">
+        <v>106</v>
+      </c>
+      <c r="C135">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>107</v>
+      </c>
+      <c r="B136" t="s">
+        <v>92</v>
+      </c>
+      <c r="C136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>108</v>
+      </c>
+      <c r="B137" t="s">
+        <v>109</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>110</v>
+      </c>
+      <c r="B138" t="s">
+        <v>92</v>
+      </c>
+      <c r="C138">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>111</v>
+      </c>
+      <c r="B139" t="s">
+        <v>112</v>
+      </c>
+      <c r="C139">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>113</v>
+      </c>
+      <c r="B140" t="s">
+        <v>92</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>114</v>
+      </c>
+      <c r="B141" t="s">
+        <v>115</v>
+      </c>
+      <c r="C141">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>116</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B142" t="s">
         <v>92</v>
       </c>
-      <c r="C119">
+      <c r="C142">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
level 2 and 3 tutorial/dialog
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D0F6E6-7CF6-404A-98C7-C2B84A2BF881}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CE313B-9DA1-4650-BE8A-486D59468893}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1725" yWindow="1740" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="290">
   <si>
     <t>Key</t>
   </si>
@@ -712,9 +712,6 @@
     <t>intro_magma_chamber_4</t>
   </si>
   <si>
-    <t>On Earth, rocks are continuously pushed upward or downward due to physical activities such as an earthquake.</t>
-  </si>
-  <si>
     <t>intro_enter_magma_cooler_1</t>
   </si>
   <si>
@@ -806,6 +803,93 @@
   </si>
   <si>
     <t>Excellent work! Now that the rocks have been submitted, we can gather more minerals to form new rocks.</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_cooler_extrusive_1</t>
+  </si>
+  <si>
+    <t>intro_enter_magma_cooler_extrusive_2</t>
+  </si>
+  <si>
+    <t>intro_extrusive_igneous_1</t>
+  </si>
+  <si>
+    <t>intro_extrusive_igneous_2</t>
+  </si>
+  <si>
+    <t>intro_extrusive_igneous_3</t>
+  </si>
+  <si>
+    <t>Just like before, we need to form three different types of rocks.</t>
+  </si>
+  <si>
+    <t>These rocks are formed when magma cools off above the Earth's surface.</t>
+  </si>
+  <si>
+    <t>This time around, we'll be forming extrusive igneous rocks.</t>
+  </si>
+  <si>
+    <t>Since these rocks cool off quicker, they don't form as much crystals as intrusive igneous rocks.</t>
+  </si>
+  <si>
+    <t>Remember to melt the minerals in the Magma Chamber, and then form the rocks in the Magma Cooler.</t>
+  </si>
+  <si>
+    <t>On Earth, rocks are continuously pushed upward or downward due to powerful forces such as an earthquake.</t>
+  </si>
+  <si>
+    <t>sediments</t>
+  </si>
+  <si>
+    <t>Sediments</t>
+  </si>
+  <si>
+    <t>intro_enter_sedimentary_1</t>
+  </si>
+  <si>
+    <t>intro_enter_sedimentary_2</t>
+  </si>
+  <si>
+    <t>For sedimentary rocks to be formed, we must first have other rocks available to erode.</t>
+  </si>
+  <si>
+    <t>Go ahead and create some igneous rocks before heading over to the Sedimentary Pit.</t>
+  </si>
+  <si>
+    <t>intro_sedimentary_1</t>
+  </si>
+  <si>
+    <t>intro_sedimentary_2</t>
+  </si>
+  <si>
+    <t>intro_sedimentary_3</t>
+  </si>
+  <si>
+    <t>rocks_require_sedimentary</t>
+  </si>
+  <si>
+    <t>Sedimentary rocks form when sediments cement together after a long period of time.</t>
+  </si>
+  <si>
+    <t>These sediments come from rocks or organics that have been broken down by weathering and erosion.</t>
+  </si>
+  <si>
+    <t>rocks_require_metamorphic</t>
+  </si>
+  <si>
+    <t>We need rocks to form metamorphic rocks. Head over to Magma Cooler or Sedimentary Pit to form some.</t>
+  </si>
+  <si>
+    <t>We need at least three rocks to form a sedimentary rock. Head over to Magma Cooler to form some.</t>
+  </si>
+  <si>
+    <t>Here in the Sedimentary Pit, we will be simulating the process of breaking down rocks into sediments, and then cementing it to form a new rock.</t>
+  </si>
+  <si>
+    <t>The result of the sedimentary rock will be based on the grain size of the sediments. So, make sure to try out different sizes!</t>
+  </si>
+  <si>
+    <t>intro_sedimentary_4</t>
   </si>
 </sst>
 </file>
@@ -1141,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,602 +1445,560 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>272</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>188</v>
+        <v>8</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>188</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B36" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>184</v>
       </c>
       <c r="B41" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B48" t="s">
-        <v>257</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>199</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
+      </c>
+      <c r="B49" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>200</v>
-      </c>
-      <c r="B50" t="s">
-        <v>210</v>
+        <v>199</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" t="s">
-        <v>256</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B53" t="s">
-        <v>206</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B55" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B56" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B58" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B59" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B60" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B61" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>231</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>254</v>
+        <v>229</v>
+      </c>
+      <c r="B62" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>231</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B64" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>238</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>239</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>240</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B68" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>241</v>
-      </c>
-      <c r="B67" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>242</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>243</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>242</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>248</v>
+      </c>
+      <c r="B71" t="s">
         <v>249</v>
       </c>
-      <c r="B70" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B72" t="s">
         <v>251</v>
       </c>
-      <c r="B71" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>259</v>
+      </c>
+      <c r="B73" t="s">
         <v>260</v>
       </c>
-      <c r="B72" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>216</v>
-      </c>
-      <c r="B73" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>218</v>
-      </c>
-      <c r="B74" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="B76" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>221</v>
+        <v>264</v>
       </c>
       <c r="B77" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>223</v>
-      </c>
-      <c r="B78" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>12</v>
-      </c>
-      <c r="B80" t="s">
-        <v>117</v>
-      </c>
-      <c r="C80">
-        <v>5</v>
+        <v>275</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>278</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81">
-        <v>0.6</v>
+        <v>282</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>279</v>
       </c>
       <c r="B82" t="s">
-        <v>117</v>
-      </c>
-      <c r="C82">
-        <v>5</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>118</v>
+        <v>280</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
+        <v>287</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
-      </c>
-      <c r="B84" t="s">
-        <v>117</v>
-      </c>
-      <c r="C84">
-        <v>5</v>
+        <v>289</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>216</v>
       </c>
       <c r="B85" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85">
-        <v>1</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
-      </c>
-      <c r="C86">
-        <v>5</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>124</v>
+        <v>235</v>
       </c>
       <c r="B87" t="s">
-        <v>125</v>
-      </c>
-      <c r="C87">
-        <v>1</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>126</v>
+        <v>281</v>
       </c>
       <c r="B88" t="s">
-        <v>117</v>
-      </c>
-      <c r="C88">
-        <v>5</v>
+        <v>286</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>127</v>
+        <v>284</v>
       </c>
       <c r="B89" t="s">
-        <v>128</v>
-      </c>
-      <c r="C89">
-        <v>0.6</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>129</v>
+        <v>225</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90">
-        <v>5</v>
+        <v>220</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>221</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
-      </c>
-      <c r="C91">
-        <v>0.6</v>
+        <v>222</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>81</v>
-      </c>
-      <c r="C92">
-        <v>5</v>
+        <v>224</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="C93">
         <v>0.6</v>
@@ -1964,10 +2006,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C94">
         <v>5</v>
@@ -1975,21 +2017,21 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B96" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C96">
         <v>5</v>
@@ -1997,21 +2039,21 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="B97" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="C97">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C98">
         <v>5</v>
@@ -2019,21 +2061,21 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="B99" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="C99">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C100">
         <v>5</v>
@@ -2041,21 +2083,21 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>25</v>
+        <v>124</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="C101">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C102">
         <v>5</v>
@@ -2063,10 +2105,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B103" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="C103">
         <v>0.6</v>
@@ -2074,10 +2116,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="B104" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
       <c r="C104">
         <v>5</v>
@@ -2085,10 +2127,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B105" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C105">
         <v>0.6</v>
@@ -2096,10 +2138,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C106">
         <v>5</v>
@@ -2107,10 +2149,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C107">
         <v>0.6</v>
@@ -2118,10 +2160,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="C108">
         <v>5</v>
@@ -2129,21 +2171,21 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C109">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C110">
         <v>5</v>
@@ -2151,21 +2193,21 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="B111" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C112">
         <v>5</v>
@@ -2173,10 +2215,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B113" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C113">
         <v>0.6</v>
@@ -2184,10 +2226,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C114">
         <v>5</v>
@@ -2195,10 +2237,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C115">
         <v>0.6</v>
@@ -2206,10 +2248,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B116" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C116">
         <v>5</v>
@@ -2217,10 +2259,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B117" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C117">
         <v>0.6</v>
@@ -2228,10 +2270,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B118" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C118">
         <v>5</v>
@@ -2239,10 +2281,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B119" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C119">
         <v>0.6</v>
@@ -2250,10 +2292,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B120" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C120">
         <v>5</v>
@@ -2261,21 +2303,21 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B121" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B122" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C122">
         <v>5</v>
@@ -2283,21 +2325,21 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B123" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C123">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B124" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C124">
         <v>5</v>
@@ -2305,10 +2347,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B125" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -2316,10 +2358,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B126" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="C126">
         <v>5</v>
@@ -2327,21 +2369,21 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="B127" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C127">
-        <v>2</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B128" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C128">
         <v>5</v>
@@ -2349,21 +2391,21 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B129" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="C129">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="B130" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C130">
         <v>5</v>
@@ -2371,10 +2413,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B131" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C131">
         <v>0.6</v>
@@ -2382,10 +2424,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="B132" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C132">
         <v>5</v>
@@ -2393,21 +2435,21 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="B133" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="C133">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="B134" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="C134">
         <v>5</v>
@@ -2415,21 +2457,21 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B135" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C135">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="B136" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C136">
         <v>5</v>
@@ -2437,21 +2479,21 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B137" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="B138" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C138">
         <v>5</v>
@@ -2459,18 +2501,18 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B139" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C139">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B140" t="s">
         <v>92</v>
@@ -2481,23 +2523,177 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B141" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C141">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B142" t="s">
         <v>92</v>
       </c>
       <c r="C142">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>96</v>
+      </c>
+      <c r="B143" t="s">
+        <v>97</v>
+      </c>
+      <c r="C143">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>98</v>
+      </c>
+      <c r="B144" t="s">
+        <v>92</v>
+      </c>
+      <c r="C144">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>99</v>
+      </c>
+      <c r="B145" t="s">
+        <v>100</v>
+      </c>
+      <c r="C145">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>101</v>
+      </c>
+      <c r="B146" t="s">
+        <v>92</v>
+      </c>
+      <c r="C146">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>102</v>
+      </c>
+      <c r="B147" t="s">
+        <v>103</v>
+      </c>
+      <c r="C147">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>104</v>
+      </c>
+      <c r="B148" t="s">
+        <v>92</v>
+      </c>
+      <c r="C148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>105</v>
+      </c>
+      <c r="B149" t="s">
+        <v>106</v>
+      </c>
+      <c r="C149">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>107</v>
+      </c>
+      <c r="B150" t="s">
+        <v>92</v>
+      </c>
+      <c r="C150">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>108</v>
+      </c>
+      <c r="B151" t="s">
+        <v>109</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>110</v>
+      </c>
+      <c r="B152" t="s">
+        <v>92</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>111</v>
+      </c>
+      <c r="B153" t="s">
+        <v>112</v>
+      </c>
+      <c r="C153">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>113</v>
+      </c>
+      <c r="B154" t="s">
+        <v>92</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>114</v>
+      </c>
+      <c r="B155" t="s">
+        <v>115</v>
+      </c>
+      <c r="C155">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>116</v>
+      </c>
+      <c r="B156" t="s">
+        <v>92</v>
+      </c>
+      <c r="C156">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some tweaks, release build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071B3CE-89DB-4AEE-AEC4-055CC1D90C52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CD4F23-DAC5-492E-9E5D-2C9B7D72CFF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2310" yWindow="1050" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
   <si>
     <t>Key</t>
   </si>
@@ -586,9 +586,6 @@
     <t>Welcome to Super Gnomatic Rock Cycler!</t>
   </si>
   <si>
-    <t>intro_2</t>
-  </si>
-  <si>
     <t>intro_3</t>
   </si>
   <si>
@@ -619,12 +616,6 @@
     <t>Press the Spacebar to enter.</t>
   </si>
   <si>
-    <t>Rocks are made up of minerals.</t>
-  </si>
-  <si>
-    <t>Depending on the minerals and how it was formed, a rock can have distinct characteristics.</t>
-  </si>
-  <si>
     <t>instruction_jump</t>
   </si>
   <si>
@@ -745,12 +736,6 @@
     <t>Now that you have some minerals, it's time to melt them down into magma.</t>
   </si>
   <si>
-    <t>We'll look into more details on the different types of rocks later.</t>
-  </si>
-  <si>
-    <t>We'll be learning about the various processes of forming rocks.</t>
-  </si>
-  <si>
     <t>For now, let's go ahead and gather some minerals!</t>
   </si>
   <si>
@@ -1130,6 +1115,15 @@
   </si>
   <si>
     <t>A metamorphic rock made up of platy crystals formed from clay that has undergone heat and pressure.</t>
+  </si>
+  <si>
+    <t>We'll look into more details later.</t>
+  </si>
+  <si>
+    <t>Rocks are made up of minerals that formed, and bonded together.</t>
+  </si>
+  <si>
+    <t>Based on how a rock is formed, it is categorized into one of these groups: igneous, sedimentary, metamorphic.</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,10 +1665,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" t="s">
         <v>194</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,10 +1689,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,26 +1768,26 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B34" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B35" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1814,10 +1808,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1862,10 +1856,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B44" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1944,16 +1938,16 @@
       <c r="A54" t="s">
         <v>188</v>
       </c>
-      <c r="B54" t="s">
-        <v>242</v>
+      <c r="B54" s="2" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>199</v>
+      <c r="B55" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1961,7 +1955,7 @@
         <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1969,7 +1963,7 @@
         <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1977,1209 +1971,1201 @@
         <v>192</v>
       </c>
       <c r="B58" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B60" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B61" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B62" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B66" t="s">
-        <v>336</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>219</v>
-      </c>
-      <c r="B67" t="s">
-        <v>226</v>
+        <v>217</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>239</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>221</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>325</v>
+        <v>219</v>
+      </c>
+      <c r="B69" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>222</v>
-      </c>
-      <c r="B70" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>228</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
+      </c>
+      <c r="B72" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>229</v>
-      </c>
-      <c r="B73" t="s">
-        <v>326</v>
+        <v>227</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>327</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>231</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
+      </c>
+      <c r="B75" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>234</v>
+      </c>
+      <c r="B76" t="s">
         <v>235</v>
-      </c>
-      <c r="B76" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>244</v>
-      </c>
-      <c r="B78" t="s">
-        <v>245</v>
+        <v>241</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>246</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>328</v>
+        <v>242</v>
+      </c>
+      <c r="B79" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B81" t="s">
-        <v>251</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>249</v>
-      </c>
-      <c r="B82" t="s">
-        <v>333</v>
+        <v>245</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>250</v>
-      </c>
-      <c r="B83" s="2" t="s">
         <v>252</v>
+      </c>
+      <c r="B83" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>257</v>
-      </c>
-      <c r="B84" t="s">
-        <v>332</v>
+        <v>253</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>258</v>
-      </c>
-      <c r="B85" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B85" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B86" t="s">
-        <v>264</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B87" t="s">
-        <v>331</v>
+        <v>263</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>262</v>
-      </c>
-      <c r="B88" t="s">
-        <v>268</v>
+        <v>265</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>274</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
+      </c>
+      <c r="B92" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>275</v>
-      </c>
-      <c r="B93" t="s">
-        <v>330</v>
+        <v>271</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>276</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
+      </c>
+      <c r="B94" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>279</v>
-      </c>
-      <c r="B95" t="s">
-        <v>322</v>
+        <v>275</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>280</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>287</v>
+        <v>276</v>
+      </c>
+      <c r="B96" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>281</v>
-      </c>
-      <c r="B97" t="s">
-        <v>286</v>
+        <v>277</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C103">
-        <v>5</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>292</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>293</v>
+        <v>203</v>
+      </c>
+      <c r="B107" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" t="s">
         <v>206</v>
-      </c>
-      <c r="B108" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>208</v>
-      </c>
-      <c r="B109" t="s">
-        <v>209</v>
+        <v>291</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>308</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>303</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>304</v>
+        <v>221</v>
+      </c>
+      <c r="B114" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>258</v>
       </c>
       <c r="B115" t="s">
-        <v>225</v>
+        <v>262</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B116" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>265</v>
+        <v>212</v>
       </c>
       <c r="B117" t="s">
-        <v>266</v>
+        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B118" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>210</v>
+      </c>
+      <c r="B119" t="s">
         <v>211</v>
-      </c>
-      <c r="B119" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>213</v>
+        <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
+        <v>11</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>10</v>
-      </c>
-      <c r="B121" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="C121">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>12</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>343</v>
+        <v>9</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
       </c>
       <c r="C122">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B123" t="s">
-        <v>13</v>
+        <v>339</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="B124" t="s">
-        <v>344</v>
+        <v>109</v>
       </c>
       <c r="C124">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>340</v>
       </c>
       <c r="C125">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B126" t="s">
-        <v>345</v>
+        <v>112</v>
       </c>
       <c r="C126">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B127" t="s">
-        <v>112</v>
+        <v>341</v>
       </c>
       <c r="C127">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B128" t="s">
-        <v>346</v>
+        <v>115</v>
       </c>
       <c r="C128">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
+        <v>342</v>
       </c>
       <c r="C129">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B130" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
       <c r="C130">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
+        <v>343</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="B132" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C132">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B133" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C133">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B134" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="C134">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>76</v>
-      </c>
-      <c r="B135" t="s">
-        <v>334</v>
+        <v>77</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>346</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>77</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>351</v>
+        <v>15</v>
+      </c>
+      <c r="B136" t="s">
+        <v>16</v>
       </c>
       <c r="C136">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>347</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B138" t="s">
-        <v>352</v>
+        <v>19</v>
       </c>
       <c r="C138">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B139" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B140" t="s">
-        <v>337</v>
+        <v>22</v>
       </c>
       <c r="C140">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>22</v>
+        <v>348</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B142" t="s">
-        <v>353</v>
+        <v>25</v>
       </c>
       <c r="C142">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>336</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>341</v>
+        <v>34</v>
       </c>
       <c r="C144">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B145" t="s">
-        <v>34</v>
+        <v>349</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B146" t="s">
-        <v>354</v>
+        <v>37</v>
       </c>
       <c r="C146">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B147" t="s">
-        <v>37</v>
+        <v>350</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B148" t="s">
-        <v>355</v>
+        <v>39</v>
       </c>
       <c r="C148">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>40</v>
-      </c>
-      <c r="B149" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>41</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>356</v>
+        <v>42</v>
+      </c>
+      <c r="B150" t="s">
+        <v>43</v>
       </c>
       <c r="C150">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>43</v>
+        <v>352</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B152" t="s">
-        <v>357</v>
+        <v>79</v>
       </c>
       <c r="C152">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B153" t="s">
-        <v>79</v>
+        <v>353</v>
       </c>
       <c r="C153">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B154" t="s">
-        <v>358</v>
+        <v>46</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>45</v>
-      </c>
-      <c r="B155" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="C155">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>47</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>359</v>
+        <v>48</v>
+      </c>
+      <c r="B156" t="s">
+        <v>49</v>
       </c>
       <c r="C156">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B157" t="s">
-        <v>49</v>
+        <v>333</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B158" t="s">
-        <v>338</v>
+        <v>52</v>
       </c>
       <c r="C158">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>51</v>
-      </c>
-      <c r="B159" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>356</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>53</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>361</v>
+        <v>54</v>
+      </c>
+      <c r="B160" t="s">
+        <v>55</v>
       </c>
       <c r="C160">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>54</v>
-      </c>
-      <c r="B161" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>56</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>360</v>
+        <v>57</v>
+      </c>
+      <c r="B162" t="s">
+        <v>58</v>
       </c>
       <c r="C162">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B163" t="s">
-        <v>58</v>
+        <v>357</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B164" t="s">
-        <v>362</v>
+        <v>61</v>
       </c>
       <c r="C164">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>60</v>
-      </c>
-      <c r="B165" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>358</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>62</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>363</v>
+        <v>81</v>
+      </c>
+      <c r="B166" t="s">
+        <v>82</v>
       </c>
       <c r="C166">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>82</v>
+        <v>359</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B168" t="s">
-        <v>364</v>
+        <v>85</v>
       </c>
       <c r="C168">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>84</v>
-      </c>
-      <c r="B169" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>86</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>365</v>
+        <v>87</v>
+      </c>
+      <c r="B170" t="s">
+        <v>88</v>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B171" t="s">
-        <v>88</v>
+        <v>335</v>
       </c>
       <c r="C171">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B172" t="s">
-        <v>340</v>
+        <v>91</v>
       </c>
       <c r="C172">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B173" t="s">
-        <v>91</v>
+        <v>334</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B174" t="s">
-        <v>339</v>
+        <v>94</v>
       </c>
       <c r="C174">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B175" t="s">
-        <v>94</v>
+        <v>361</v>
       </c>
       <c r="C175">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B176" t="s">
-        <v>366</v>
+        <v>97</v>
       </c>
       <c r="C176">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>96</v>
-      </c>
-      <c r="B177" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>98</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>368</v>
+        <v>99</v>
+      </c>
+      <c r="B178" t="s">
+        <v>100</v>
       </c>
       <c r="C178">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B179" t="s">
-        <v>100</v>
+        <v>337</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B180" t="s">
-        <v>342</v>
+        <v>103</v>
       </c>
       <c r="C180">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>102</v>
-      </c>
-      <c r="B181" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>364</v>
       </c>
       <c r="C181">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>104</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>369</v>
+        <v>105</v>
+      </c>
+      <c r="B182" t="s">
+        <v>106</v>
       </c>
       <c r="C182">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>105</v>
-      </c>
-      <c r="B183" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>362</v>
       </c>
       <c r="C183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>107</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C184">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to unity 2019, text update based on review
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CD4F23-DAC5-492E-9E5D-2C9B7D72CFF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084256D-D6E9-4B20-81FB-7E8CC092793D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1050" windowWidth="21600" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -763,9 +763,6 @@
     <t>This time around, we'll be forming extrusive igneous rocks.</t>
   </si>
   <si>
-    <t>Since these rocks cool off quicker, they don't form as much crystals as intrusive igneous rocks.</t>
-  </si>
-  <si>
     <t>Remember to melt the minerals in the Magma Chamber, and then form the rocks in the Magma Cooler.</t>
   </si>
   <si>
@@ -982,15 +979,6 @@
     <t>COMPLETE</t>
   </si>
   <si>
-    <t>If you notice at the very top, we need to form at least three different types of igneous rocks.</t>
-  </si>
-  <si>
-    <t>Intrusive igneous rocks are formed when magma cools off below the Earth’s surface.</t>
-  </si>
-  <si>
-    <t>Try to form three different types of rocks based on how long the magma cools.</t>
-  </si>
-  <si>
     <t>Just like before, we need to form three different types of igneous rocks.</t>
   </si>
   <si>
@@ -1000,24 +988,12 @@
     <t>For example, plants and trees that were buried for millions of years can turn into coal.</t>
   </si>
   <si>
-    <t>These sediments come from any type of rocks, or certain organics that have been broken down by weathering and erosion.</t>
-  </si>
-  <si>
     <t>For sedimentary rocks to be formed, we must first have rocks available to break down into sediments.</t>
   </si>
   <si>
-    <t>These rocks are formed when magma cools off above the Earth's surface. For example: when a volcano erupts.</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
-    <t>When rocks are pushed deep enough into the Earth, where temperature can reach its melting point, it will become magma.</t>
-  </si>
-  <si>
-    <t>Here in the Magma Chamber, we will simulate the process of melting rocks to magma.</t>
-  </si>
-  <si>
     <t>A coarse-grained igneous rock. Its color is usually black or dark green.</t>
   </si>
   <si>
@@ -1078,9 +1054,6 @@
     <t>An extrusive igneous rock that is usually pink or gray in color.</t>
   </si>
   <si>
-    <t>A fine-grained igneous rock that is usually black in color. These are commonly found in ocean floor.</t>
-  </si>
-  <si>
     <t>An igneous rock that forms when lava is cooled rapidly, resulting in its black glassy feature.</t>
   </si>
   <si>
@@ -1120,10 +1093,37 @@
     <t>We'll look into more details later.</t>
   </si>
   <si>
-    <t>Rocks are made up of minerals that formed, and bonded together.</t>
-  </si>
-  <si>
-    <t>Based on how a rock is formed, it is categorized into one of these groups: igneous, sedimentary, metamorphic.</t>
+    <t>Rocks are made up of minerals that formed and bonded together.</t>
+  </si>
+  <si>
+    <t>Based on how it is formed, every rock is categorized into one of these groups: igneous, sedimentary, metamorphic.</t>
+  </si>
+  <si>
+    <t>When a rock is pushed deep enough into the Earth, temperatures can reach its melting point and melt the rock. When the rock melts, it will become magma.</t>
+  </si>
+  <si>
+    <t>Here in the Magma Chamber, we will simulate the process of melting rocks into magma.</t>
+  </si>
+  <si>
+    <t>If you'll notice the bar at the very top, you'll see that we need to form at least three different types of igneous rocks.</t>
+  </si>
+  <si>
+    <t>These rocks are formed when magma cools above the Earth's surface. For example: after a volcano erupts.</t>
+  </si>
+  <si>
+    <t>Intrusive igneous rocks are formed when magma cools below the Earth’s surface.</t>
+  </si>
+  <si>
+    <t>Try to form three different types of rocks based on how long the magma takes to cool.</t>
+  </si>
+  <si>
+    <t>Since these rocks cool off faster, they don't form as many crystals as intrusive igneous rocks.</t>
+  </si>
+  <si>
+    <t>A fine-grained igneous rock that is usually black in color. These are commonly found on the ocean floor.</t>
+  </si>
+  <si>
+    <t>These sediments come from any type of rocks, or certain organic materials that have been broken down by weathering and erosion.</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,10 +1689,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" t="s">
         <v>250</v>
-      </c>
-      <c r="B25" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,26 +1768,26 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,10 +1808,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" t="s">
         <v>300</v>
-      </c>
-      <c r="B38" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1856,10 +1856,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>317</v>
+      </c>
+      <c r="B44" t="s">
         <v>318</v>
-      </c>
-      <c r="B44" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1939,7 +1939,7 @@
         <v>188</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1955,7 +1955,7 @@
         <v>190</v>
       </c>
       <c r="B56" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2011,7 +2011,7 @@
         <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,7 +2019,7 @@
         <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>330</v>
+        <v>359</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2027,7 +2027,7 @@
         <v>215</v>
       </c>
       <c r="B65" t="s">
-        <v>331</v>
+        <v>360</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2051,7 @@
         <v>218</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>320</v>
+        <v>361</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
         <v>226</v>
       </c>
       <c r="B72" t="s">
-        <v>321</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>227</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>322</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>241</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>242</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
         <v>244</v>
       </c>
       <c r="B81" t="s">
-        <v>328</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2163,167 +2163,167 @@
         <v>245</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>247</v>
+        <v>365</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B83" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>252</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B85" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B86" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B94" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B96" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>308</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>310</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>314</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="C102">
         <v>5</v>
@@ -2331,34 +2331,34 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>282</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>288</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>284</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>286</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,42 +2379,42 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>290</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>292</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>297</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2427,18 +2427,18 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B115" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>259</v>
+      </c>
+      <c r="B116" t="s">
         <v>260</v>
-      </c>
-      <c r="B116" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2481,7 +2481,7 @@
         <v>12</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C121">
         <v>5</v>
@@ -2503,7 +2503,7 @@
         <v>14</v>
       </c>
       <c r="B123" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C123">
         <v>5</v>
@@ -2525,7 +2525,7 @@
         <v>110</v>
       </c>
       <c r="B125" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C125">
         <v>5</v>
@@ -2547,7 +2547,7 @@
         <v>113</v>
       </c>
       <c r="B127" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C127">
         <v>5</v>
@@ -2569,7 +2569,7 @@
         <v>116</v>
       </c>
       <c r="B129" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C129">
         <v>5</v>
@@ -2591,7 +2591,7 @@
         <v>119</v>
       </c>
       <c r="B131" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C131">
         <v>5</v>
@@ -2602,7 +2602,7 @@
         <v>74</v>
       </c>
       <c r="B132" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -2613,7 +2613,7 @@
         <v>75</v>
       </c>
       <c r="B133" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C133">
         <v>5</v>
@@ -2624,7 +2624,7 @@
         <v>76</v>
       </c>
       <c r="B134" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -2635,7 +2635,7 @@
         <v>77</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C135">
         <v>5</v>
@@ -2657,7 +2657,7 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C137">
         <v>5</v>
@@ -2679,7 +2679,7 @@
         <v>20</v>
       </c>
       <c r="B139" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C139">
         <v>5</v>
@@ -2701,7 +2701,7 @@
         <v>23</v>
       </c>
       <c r="B141" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C141">
         <v>5</v>
@@ -2723,7 +2723,7 @@
         <v>26</v>
       </c>
       <c r="B143" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C143">
         <v>5</v>
@@ -2745,7 +2745,7 @@
         <v>35</v>
       </c>
       <c r="B145" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C145">
         <v>5</v>
@@ -2767,7 +2767,7 @@
         <v>38</v>
       </c>
       <c r="B147" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C147">
         <v>5</v>
@@ -2789,7 +2789,7 @@
         <v>41</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -2811,7 +2811,7 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
       <c r="C151">
         <v>5</v>
@@ -2833,7 +2833,7 @@
         <v>80</v>
       </c>
       <c r="B153" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C153">
         <v>5</v>
@@ -2855,7 +2855,7 @@
         <v>47</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C155">
         <v>5</v>
@@ -2877,7 +2877,7 @@
         <v>50</v>
       </c>
       <c r="B157" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C157">
         <v>5</v>
@@ -2899,7 +2899,7 @@
         <v>53</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C159">
         <v>5</v>
@@ -2921,7 +2921,7 @@
         <v>56</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C161">
         <v>5</v>
@@ -2943,7 +2943,7 @@
         <v>59</v>
       </c>
       <c r="B163" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="C163">
         <v>5</v>
@@ -2965,7 +2965,7 @@
         <v>62</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="C165">
         <v>5</v>
@@ -2987,7 +2987,7 @@
         <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C167">
         <v>5</v>
@@ -3009,7 +3009,7 @@
         <v>86</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C169">
         <v>5</v>
@@ -3031,7 +3031,7 @@
         <v>89</v>
       </c>
       <c r="B171" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C171">
         <v>5</v>
@@ -3053,7 +3053,7 @@
         <v>92</v>
       </c>
       <c r="B173" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C173">
         <v>5</v>
@@ -3075,7 +3075,7 @@
         <v>95</v>
       </c>
       <c r="B175" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C175">
         <v>5</v>
@@ -3097,7 +3097,7 @@
         <v>98</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="C177">
         <v>5</v>
@@ -3119,7 +3119,7 @@
         <v>101</v>
       </c>
       <c r="B179" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C179">
         <v>5</v>
@@ -3141,7 +3141,7 @@
         <v>104</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="C181">
         <v>5</v>
@@ -3163,7 +3163,7 @@
         <v>107</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C183">
         <v>5</v>

</xml_diff>

<commit_message>
rock cycle ui, show arrows to indicate where to go in hub
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E084256D-D6E9-4B20-81FB-7E8CC092793D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177451E7-4849-4B56-8202-8AD833449D55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
   <si>
     <t>Key</t>
   </si>
@@ -1124,6 +1124,12 @@
   </si>
   <si>
     <t>These sediments come from any type of rocks, or certain organic materials that have been broken down by weathering and erosion.</t>
+  </si>
+  <si>
+    <t>THE ROCK CYCLE</t>
+  </si>
+  <si>
+    <t>rock_cycle_title</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,1332 +1846,1340 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>369</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>368</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>317</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
-        <v>318</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>172</v>
+        <v>317</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>187</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>188</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>357</v>
+        <v>185</v>
+      </c>
+      <c r="B54" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>189</v>
-      </c>
-      <c r="B55" t="s">
-        <v>358</v>
+        <v>188</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B56" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B57" t="s">
-        <v>238</v>
+        <v>356</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B59" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B61" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B63" t="s">
-        <v>248</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B64" t="s">
-        <v>359</v>
+        <v>248</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
-        <v>223</v>
+        <v>360</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>217</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="B67" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>361</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>219</v>
-      </c>
-      <c r="B69" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>224</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
+      </c>
+      <c r="B70" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>226</v>
-      </c>
-      <c r="B72" t="s">
-        <v>363</v>
+        <v>225</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>227</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>364</v>
+        <v>226</v>
+      </c>
+      <c r="B73" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>231</v>
+        <v>364</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>232</v>
-      </c>
-      <c r="B75" t="s">
-        <v>233</v>
+        <v>228</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B76" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>241</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>319</v>
+        <v>239</v>
+      </c>
+      <c r="B78" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>242</v>
-      </c>
-      <c r="B79" t="s">
-        <v>247</v>
+        <v>241</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B81" t="s">
-        <v>362</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>245</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>365</v>
+        <v>244</v>
+      </c>
+      <c r="B82" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>251</v>
-      </c>
-      <c r="B83" t="s">
-        <v>322</v>
+        <v>245</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>252</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
+      </c>
+      <c r="B84" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>254</v>
-      </c>
-      <c r="B85" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B86" t="s">
-        <v>367</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B87" t="s">
-        <v>262</v>
+        <v>367</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>264</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
+      </c>
+      <c r="B88" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>271</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>269</v>
-      </c>
-      <c r="B92" t="s">
-        <v>321</v>
+        <v>268</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>270</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
+      </c>
+      <c r="B93" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>273</v>
-      </c>
-      <c r="B94" t="s">
-        <v>316</v>
+        <v>270</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>274</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
+      </c>
+      <c r="B95" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>275</v>
-      </c>
-      <c r="B96" t="s">
-        <v>280</v>
+        <v>274</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>276</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+      <c r="B97" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C102">
-        <v>5</v>
+        <v>313</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>283</v>
+        <v>315</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>203</v>
-      </c>
-      <c r="B107" t="s">
-        <v>204</v>
+        <v>286</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B108" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>290</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>291</v>
+        <v>205</v>
+      </c>
+      <c r="B109" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>221</v>
-      </c>
-      <c r="B114" t="s">
-        <v>222</v>
+        <v>297</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="B115" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B116" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="B117" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B118" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B119" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="B120" t="s">
-        <v>11</v>
-      </c>
-      <c r="C120">
-        <v>1</v>
+        <v>211</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>12</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>330</v>
+        <v>10</v>
+      </c>
+      <c r="B121" t="s">
+        <v>11</v>
       </c>
       <c r="C121">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="C122">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>331</v>
+        <v>13</v>
       </c>
       <c r="C123">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>331</v>
       </c>
       <c r="C124">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B125" t="s">
-        <v>332</v>
+        <v>109</v>
       </c>
       <c r="C125">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B126" t="s">
-        <v>112</v>
+        <v>332</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B127" t="s">
-        <v>333</v>
+        <v>112</v>
       </c>
       <c r="C127">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>333</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B129" t="s">
-        <v>334</v>
+        <v>115</v>
       </c>
       <c r="C129">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B130" t="s">
-        <v>118</v>
+        <v>334</v>
       </c>
       <c r="C130">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B131" t="s">
-        <v>335</v>
+        <v>118</v>
       </c>
       <c r="C131">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B133" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C133">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B134" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>77</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>338</v>
+        <v>76</v>
+      </c>
+      <c r="B135" t="s">
+        <v>323</v>
       </c>
       <c r="C135">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>15</v>
-      </c>
-      <c r="B136" t="s">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>338</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B137" t="s">
-        <v>339</v>
+        <v>16</v>
       </c>
       <c r="C137">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>19</v>
+        <v>339</v>
       </c>
       <c r="C138">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B139" t="s">
-        <v>324</v>
+        <v>19</v>
       </c>
       <c r="C139">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>22</v>
+        <v>324</v>
       </c>
       <c r="C140">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>340</v>
+        <v>22</v>
       </c>
       <c r="C141">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>340</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B143" t="s">
-        <v>328</v>
+        <v>25</v>
       </c>
       <c r="C143">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B144" t="s">
-        <v>34</v>
+        <v>328</v>
       </c>
       <c r="C144">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B145" t="s">
-        <v>341</v>
+        <v>34</v>
       </c>
       <c r="C145">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B146" t="s">
-        <v>37</v>
+        <v>341</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B147" t="s">
-        <v>342</v>
+        <v>37</v>
       </c>
       <c r="C147">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B148" t="s">
-        <v>39</v>
+        <v>342</v>
       </c>
       <c r="C148">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>41</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>343</v>
+        <v>40</v>
+      </c>
+      <c r="B149" t="s">
+        <v>39</v>
       </c>
       <c r="C149">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>42</v>
-      </c>
-      <c r="B150" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="C150">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B151" t="s">
-        <v>366</v>
+        <v>43</v>
       </c>
       <c r="C151">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B152" t="s">
-        <v>79</v>
+        <v>366</v>
       </c>
       <c r="C152">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>344</v>
+        <v>79</v>
       </c>
       <c r="C153">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B154" t="s">
-        <v>46</v>
+        <v>344</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>47</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>345</v>
+        <v>45</v>
+      </c>
+      <c r="B155" t="s">
+        <v>46</v>
       </c>
       <c r="C155">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>48</v>
-      </c>
-      <c r="B156" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="C156">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>325</v>
+        <v>49</v>
       </c>
       <c r="C157">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B158" t="s">
-        <v>52</v>
+        <v>325</v>
       </c>
       <c r="C158">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>53</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>347</v>
+        <v>51</v>
+      </c>
+      <c r="B159" t="s">
+        <v>52</v>
       </c>
       <c r="C159">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>54</v>
-      </c>
-      <c r="B160" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="C160">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>56</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>346</v>
+        <v>54</v>
+      </c>
+      <c r="B161" t="s">
+        <v>55</v>
       </c>
       <c r="C161">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>57</v>
-      </c>
-      <c r="B162" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>346</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B163" t="s">
-        <v>348</v>
+        <v>58</v>
       </c>
       <c r="C163">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B164" t="s">
-        <v>61</v>
+        <v>348</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>62</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>349</v>
+        <v>60</v>
+      </c>
+      <c r="B165" t="s">
+        <v>61</v>
       </c>
       <c r="C165">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>81</v>
-      </c>
-      <c r="B166" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="C166">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B167" t="s">
-        <v>350</v>
+        <v>82</v>
       </c>
       <c r="C167">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B168" t="s">
-        <v>85</v>
+        <v>350</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>86</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>351</v>
+        <v>84</v>
+      </c>
+      <c r="B169" t="s">
+        <v>85</v>
       </c>
       <c r="C169">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>87</v>
-      </c>
-      <c r="B170" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>351</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B171" t="s">
-        <v>327</v>
+        <v>88</v>
       </c>
       <c r="C171">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B172" t="s">
-        <v>91</v>
+        <v>327</v>
       </c>
       <c r="C172">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B173" t="s">
-        <v>326</v>
+        <v>91</v>
       </c>
       <c r="C173">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B174" t="s">
-        <v>94</v>
+        <v>326</v>
       </c>
       <c r="C174">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B175" t="s">
-        <v>352</v>
+        <v>94</v>
       </c>
       <c r="C175">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B176" t="s">
-        <v>97</v>
+        <v>352</v>
       </c>
       <c r="C176">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>98</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>354</v>
+        <v>96</v>
+      </c>
+      <c r="B177" t="s">
+        <v>97</v>
       </c>
       <c r="C177">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>99</v>
-      </c>
-      <c r="B178" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>354</v>
       </c>
       <c r="C178">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B179" t="s">
-        <v>329</v>
+        <v>100</v>
       </c>
       <c r="C179">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B180" t="s">
-        <v>103</v>
+        <v>329</v>
       </c>
       <c r="C180">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>104</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>355</v>
+        <v>102</v>
+      </c>
+      <c r="B181" t="s">
+        <v>103</v>
       </c>
       <c r="C181">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>105</v>
-      </c>
-      <c r="B182" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>355</v>
       </c>
       <c r="C182">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>105</v>
+      </c>
+      <c r="B183" t="s">
+        <v>106</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>107</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B184" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="C183">
+      <c r="C184">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more information on rock cycle and tutorial
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177451E7-4849-4B56-8202-8AD833449D55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22259BEF-8B09-40A8-BF9A-AABE3D693F02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
   <si>
     <t>Key</t>
   </si>
@@ -703,21 +703,12 @@
     <t>intro_intrusive_igneous_3</t>
   </si>
   <si>
-    <t>intro_intrusive_igneous_4</t>
-  </si>
-  <si>
-    <t>intrusive_igneous_instruction</t>
-  </si>
-  <si>
     <t>There are two ways for igneous rocks to form: intrusive or extrusive.</t>
   </si>
   <si>
     <t>For now, we will form intrusive igneous rocks.</t>
   </si>
   <si>
-    <t>Press the Spacebar (or click STOP) to end the cooling process.</t>
-  </si>
-  <si>
     <t>submit_instruction_1</t>
   </si>
   <si>
@@ -796,9 +787,6 @@
     <t>rocks_require_sedimentary</t>
   </si>
   <si>
-    <t>Sedimentary rocks form when sediments cement together after a long period of time.</t>
-  </si>
-  <si>
     <t>rocks_require_metamorphic</t>
   </si>
   <si>
@@ -1105,31 +1093,127 @@
     <t>Here in the Magma Chamber, we will simulate the process of melting rocks into magma.</t>
   </si>
   <si>
-    <t>If you'll notice the bar at the very top, you'll see that we need to form at least three different types of igneous rocks.</t>
-  </si>
-  <si>
     <t>These rocks are formed when magma cools above the Earth's surface. For example: after a volcano erupts.</t>
   </si>
   <si>
     <t>Intrusive igneous rocks are formed when magma cools below the Earth’s surface.</t>
   </si>
   <si>
-    <t>Try to form three different types of rocks based on how long the magma takes to cool.</t>
-  </si>
-  <si>
     <t>Since these rocks cool off faster, they don't form as many crystals as intrusive igneous rocks.</t>
   </si>
   <si>
     <t>A fine-grained igneous rock that is usually black in color. These are commonly found on the ocean floor.</t>
   </si>
   <si>
-    <t>These sediments come from any type of rocks, or certain organic materials that have been broken down by weathering and erosion.</t>
-  </si>
-  <si>
     <t>THE ROCK CYCLE</t>
   </si>
   <si>
     <t>rock_cycle_title</t>
+  </si>
+  <si>
+    <t>intro_magma_rock_cycle_1</t>
+  </si>
+  <si>
+    <t>In this part of the rock cycle, we will be looking at rocks melting to magma.</t>
+  </si>
+  <si>
+    <t>intro_magma_rock_cycle_2</t>
+  </si>
+  <si>
+    <t>instruction_exit</t>
+  </si>
+  <si>
+    <t>Press this button to exit and proceed.</t>
+  </si>
+  <si>
+    <t>instruction_exit_criteria_met</t>
+  </si>
+  <si>
+    <t>enter_magma_chamber</t>
+  </si>
+  <si>
+    <t>ENTER MAGMA CHAMBER</t>
+  </si>
+  <si>
+    <t>enter_magma_cooler</t>
+  </si>
+  <si>
+    <t>ENTER MAGMA COOLER</t>
+  </si>
+  <si>
+    <t>enter_sedimentary_pit</t>
+  </si>
+  <si>
+    <t>ENTER SEDIMENTARY PIT</t>
+  </si>
+  <si>
+    <t>intro_igneous_rock_cycle_1</t>
+  </si>
+  <si>
+    <t>For this rock cycle, we will be looking at magma cooling off, and solidifying to a rock.</t>
+  </si>
+  <si>
+    <t>intro_igneous_cool_off_1</t>
+  </si>
+  <si>
+    <t>intro_igneous_cool_off_2</t>
+  </si>
+  <si>
+    <t>When magma is pushed upwards due to the flow of energy inside the Earth, it will eventually cool off and crystalize into various minerals.</t>
+  </si>
+  <si>
+    <t>During crystalization, various minerals will form and bond together, eventually becoming an igneous rock.</t>
+  </si>
+  <si>
+    <t>Press spacebar, or click on this button to proceed.</t>
+  </si>
+  <si>
+    <t>You now have the necessary rock types! Press this button to exit and proceed.</t>
+  </si>
+  <si>
+    <t>intruction_press_proceed</t>
+  </si>
+  <si>
+    <t>As you can see, all rocks eventually melt down to magma.</t>
+  </si>
+  <si>
+    <t>intro_sedimentary_rock_cycle_1</t>
+  </si>
+  <si>
+    <t>Sediments come from any type of rocks, or certain organic materials that have been broken down by weathering and erosion.</t>
+  </si>
+  <si>
+    <t>After a long period of time, sediments that have accumulated into an area will compact and cement to form sedimentary rocks.</t>
+  </si>
+  <si>
+    <t>For this rock cycle, we will see how rocks are broken up to sediments, and then formed to a sedimentary rock.</t>
+  </si>
+  <si>
+    <t>intro_metamorph_rock_cycle_1</t>
+  </si>
+  <si>
+    <t>For this rock cycle, we will see how rocks are transformed into a metamorphic rock.</t>
+  </si>
+  <si>
+    <t>intro_metamorph_rock_cycle_2</t>
+  </si>
+  <si>
+    <t>As you can see, all rocks eventually sink beneath the Earth, forming into a different rock.</t>
+  </si>
+  <si>
+    <t>intro_metamorph_rock_cycle_3</t>
+  </si>
+  <si>
+    <t>And finally, sinking further to melt into magma, completing the rock cycle.</t>
+  </si>
+  <si>
+    <t>rock_criteria_not_met</t>
+  </si>
+  <si>
+    <t>You must fill up the rock slots before submitting.</t>
+  </si>
+  <si>
+    <t>If you notice the bar at the very top, you'll see that we need to form at least three different types of igneous rocks.</t>
   </si>
 </sst>
 </file>
@@ -1475,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,10 +1779,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1774,26 +1858,26 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B33" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B34" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B35" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1814,10 +1898,10 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1846,10 +1930,10 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B42" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1870,775 +1954,733 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B45" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>369</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>174</v>
+        <v>371</v>
       </c>
       <c r="B47" t="s">
-        <v>176</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>373</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>374</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>187</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>188</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>357</v>
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>358</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B57" t="s">
-        <v>356</v>
+        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>191</v>
-      </c>
-      <c r="B58" t="s">
-        <v>238</v>
+        <v>188</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>354</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>352</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B63" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B64" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>366</v>
       </c>
       <c r="B65" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>215</v>
+        <v>368</v>
       </c>
       <c r="B66" t="s">
-        <v>360</v>
+        <v>382</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="B67" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>217</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>236</v>
+        <v>201</v>
+      </c>
+      <c r="B68" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>218</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>361</v>
+        <v>363</v>
+      </c>
+      <c r="B69" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>219</v>
+        <v>365</v>
       </c>
       <c r="B70" t="s">
-        <v>220</v>
+        <v>384</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>224</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>229</v>
+        <v>213</v>
+      </c>
+      <c r="B71" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>225</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>230</v>
+        <v>214</v>
+      </c>
+      <c r="B72" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B73" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>227</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>364</v>
+        <v>216</v>
+      </c>
+      <c r="B74" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>232</v>
-      </c>
-      <c r="B76" t="s">
-        <v>233</v>
+        <v>218</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>375</v>
       </c>
       <c r="B78" t="s">
-        <v>240</v>
+        <v>376</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>241</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>319</v>
+        <v>377</v>
+      </c>
+      <c r="B79" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>242</v>
+        <v>378</v>
       </c>
       <c r="B80" t="s">
-        <v>247</v>
+        <v>380</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>243</v>
-      </c>
-      <c r="B81" t="s">
-        <v>246</v>
+        <v>224</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>244</v>
-      </c>
-      <c r="B82" t="s">
-        <v>362</v>
+        <v>225</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>245</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>365</v>
+        <v>226</v>
+      </c>
+      <c r="B83" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>383</v>
       </c>
       <c r="B84" t="s">
-        <v>322</v>
+        <v>381</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>252</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>253</v>
+        <v>229</v>
+      </c>
+      <c r="B85" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="B86" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B87" t="s">
-        <v>367</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>256</v>
-      </c>
-      <c r="B88" t="s">
-        <v>262</v>
+        <v>238</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>264</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
+      </c>
+      <c r="B89" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>265</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>267</v>
+        <v>240</v>
+      </c>
+      <c r="B90" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>266</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>320</v>
+        <v>241</v>
+      </c>
+      <c r="B91" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>268</v>
+        <v>242</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>271</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B93" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>273</v>
-      </c>
-      <c r="B95" t="s">
-        <v>316</v>
+        <v>385</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>251</v>
+      </c>
+      <c r="B96" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>253</v>
+      </c>
+      <c r="B98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>260</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>261</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>262</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>264</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>265</v>
+      </c>
+      <c r="B103" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>266</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>269</v>
+      </c>
+      <c r="B105" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>270</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>389</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>391</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>393</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>271</v>
+      </c>
+      <c r="B110" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>272</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>273</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="B97" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>276</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>277</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>308</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>310</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>312</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>314</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C103">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>282</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>288</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>284</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>286</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>203</v>
-      </c>
-      <c r="B108" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>205</v>
-      </c>
-      <c r="B109" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>290</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>307</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>292</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>221</v>
-      </c>
-      <c r="B115" t="s">
-        <v>222</v>
+        <v>308</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>257</v>
-      </c>
-      <c r="B116" t="s">
-        <v>261</v>
+        <v>310</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C116">
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>259</v>
-      </c>
-      <c r="B117" t="s">
-        <v>260</v>
+        <v>278</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>212</v>
-      </c>
-      <c r="B118" t="s">
-        <v>207</v>
+        <v>284</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>208</v>
-      </c>
-      <c r="B119" t="s">
-        <v>209</v>
+        <v>280</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>210</v>
-      </c>
-      <c r="B120" t="s">
-        <v>211</v>
+        <v>282</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
-      </c>
-      <c r="C121">
-        <v>1</v>
+        <v>204</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>12</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C122">
-        <v>5</v>
+        <v>205</v>
+      </c>
+      <c r="B122" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>9</v>
-      </c>
-      <c r="B123" t="s">
-        <v>13</v>
-      </c>
-      <c r="C123">
-        <v>1</v>
+        <v>286</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>14</v>
-      </c>
-      <c r="B124" t="s">
-        <v>331</v>
-      </c>
-      <c r="C124">
-        <v>5</v>
+        <v>303</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>108</v>
-      </c>
-      <c r="B125" t="s">
-        <v>109</v>
-      </c>
-      <c r="C125">
-        <v>1</v>
+        <v>288</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>110</v>
-      </c>
-      <c r="B126" t="s">
-        <v>332</v>
-      </c>
-      <c r="C126">
-        <v>5</v>
+        <v>292</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>111</v>
-      </c>
-      <c r="B127" t="s">
-        <v>112</v>
-      </c>
-      <c r="C127">
-        <v>1</v>
+        <v>293</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>113</v>
+        <v>221</v>
       </c>
       <c r="B128" t="s">
-        <v>333</v>
-      </c>
-      <c r="C128">
-        <v>5</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="B129" t="s">
-        <v>115</v>
-      </c>
-      <c r="C129">
-        <v>1</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>255</v>
       </c>
       <c r="B130" t="s">
-        <v>334</v>
-      </c>
-      <c r="C130">
-        <v>5</v>
+        <v>256</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>117</v>
+        <v>395</v>
       </c>
       <c r="B131" t="s">
-        <v>118</v>
-      </c>
-      <c r="C131">
-        <v>1</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="B132" t="s">
-        <v>335</v>
-      </c>
-      <c r="C132">
-        <v>5</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>74</v>
+        <v>208</v>
       </c>
       <c r="B133" t="s">
-        <v>336</v>
-      </c>
-      <c r="C133">
-        <v>1</v>
+        <v>209</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="B134" t="s">
-        <v>337</v>
-      </c>
-      <c r="C134">
-        <v>5</v>
+        <v>211</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>323</v>
+        <v>11</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -2646,10 +2688,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="C136">
         <v>5</v>
@@ -2657,10 +2699,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -2668,10 +2710,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B138" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="C138">
         <v>5</v>
@@ -2679,10 +2721,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="B139" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -2690,10 +2732,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B140" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C140">
         <v>5</v>
@@ -2701,10 +2743,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="B141" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -2712,10 +2754,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="B142" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="C142">
         <v>5</v>
@@ -2723,10 +2765,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2734,10 +2776,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="B144" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C144">
         <v>5</v>
@@ -2745,10 +2787,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="B145" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2756,10 +2798,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="B146" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C146">
         <v>5</v>
@@ -2767,10 +2809,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B147" t="s">
-        <v>37</v>
+        <v>332</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -2778,10 +2820,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B148" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C148">
         <v>5</v>
@@ -2789,10 +2831,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B149" t="s">
-        <v>39</v>
+        <v>319</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2800,10 +2842,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C150">
         <v>5</v>
@@ -2811,10 +2853,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B151" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2822,10 +2864,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>366</v>
+        <v>335</v>
       </c>
       <c r="C152">
         <v>5</v>
@@ -2833,10 +2875,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="B153" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2844,10 +2886,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B154" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -2855,10 +2897,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B155" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2866,10 +2908,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>47</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>345</v>
+        <v>23</v>
+      </c>
+      <c r="B156" t="s">
+        <v>336</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -2877,10 +2919,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B157" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2888,10 +2930,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="B158" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C158">
         <v>5</v>
@@ -2899,10 +2941,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2910,10 +2952,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>53</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>347</v>
+        <v>35</v>
+      </c>
+      <c r="B160" t="s">
+        <v>337</v>
       </c>
       <c r="C160">
         <v>5</v>
@@ -2921,10 +2963,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B161" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -2932,10 +2974,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>56</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>346</v>
+        <v>38</v>
+      </c>
+      <c r="B162" t="s">
+        <v>338</v>
       </c>
       <c r="C162">
         <v>5</v>
@@ -2943,10 +2985,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B163" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2954,10 +2996,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>59</v>
-      </c>
-      <c r="B164" t="s">
-        <v>348</v>
+        <v>41</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="C164">
         <v>5</v>
@@ -2965,10 +3007,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B165" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -2976,10 +3018,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>62</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>349</v>
+        <v>44</v>
+      </c>
+      <c r="B166" t="s">
+        <v>360</v>
       </c>
       <c r="C166">
         <v>5</v>
@@ -2987,10 +3029,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B167" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -2998,10 +3040,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B168" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C168">
         <v>5</v>
@@ -3009,21 +3051,21 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="B169" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C170">
         <v>5</v>
@@ -3031,10 +3073,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="B171" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -3042,10 +3084,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B172" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C172">
         <v>5</v>
@@ -3053,10 +3095,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="B173" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -3064,10 +3106,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>92</v>
-      </c>
-      <c r="B174" t="s">
-        <v>326</v>
+        <v>53</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="C174">
         <v>5</v>
@@ -3075,21 +3117,21 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B175" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="C175">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>95</v>
-      </c>
-      <c r="B176" t="s">
-        <v>352</v>
+        <v>56</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>342</v>
       </c>
       <c r="C176">
         <v>5</v>
@@ -3097,10 +3139,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B177" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3108,10 +3150,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>98</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>354</v>
+        <v>59</v>
+      </c>
+      <c r="B178" t="s">
+        <v>344</v>
       </c>
       <c r="C178">
         <v>5</v>
@@ -3119,10 +3161,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="B179" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -3130,10 +3172,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>101</v>
-      </c>
-      <c r="B180" t="s">
-        <v>329</v>
+        <v>62</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="C180">
         <v>5</v>
@@ -3141,10 +3183,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B181" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -3152,10 +3194,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>104</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>355</v>
+        <v>83</v>
+      </c>
+      <c r="B182" t="s">
+        <v>346</v>
       </c>
       <c r="C182">
         <v>5</v>
@@ -3163,23 +3205,177 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B183" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>86</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C184">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>87</v>
+      </c>
+      <c r="B185" t="s">
+        <v>88</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>89</v>
+      </c>
+      <c r="B186" t="s">
+        <v>323</v>
+      </c>
+      <c r="C186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>90</v>
+      </c>
+      <c r="B187" t="s">
+        <v>91</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>92</v>
+      </c>
+      <c r="B188" t="s">
+        <v>322</v>
+      </c>
+      <c r="C188">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>93</v>
+      </c>
+      <c r="B189" t="s">
+        <v>94</v>
+      </c>
+      <c r="C189">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>95</v>
+      </c>
+      <c r="B190" t="s">
+        <v>348</v>
+      </c>
+      <c r="C190">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>96</v>
+      </c>
+      <c r="B191" t="s">
+        <v>97</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>98</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C192">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>99</v>
+      </c>
+      <c r="B193" t="s">
+        <v>100</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>101</v>
+      </c>
+      <c r="B194" t="s">
+        <v>325</v>
+      </c>
+      <c r="C194">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>102</v>
+      </c>
+      <c r="B195" t="s">
+        <v>103</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>104</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C196">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>105</v>
+      </c>
+      <c r="B197" t="s">
+        <v>106</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>107</v>
       </c>
-      <c r="B184" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="C184">
+      <c r="B198" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C198">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a bunch of "fixes" and tweaks, new build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22259BEF-8B09-40A8-BF9A-AABE3D693F02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D42B8-A11A-4C15-96B3-D951501B74B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
   <si>
     <t>Key</t>
   </si>
@@ -1214,6 +1214,18 @@
   </si>
   <si>
     <t>If you notice the bar at the very top, you'll see that we need to form at least three different types of igneous rocks.</t>
+  </si>
+  <si>
+    <t>instruction_submit</t>
+  </si>
+  <si>
+    <t>Press the Spacebar to submit.</t>
+  </si>
+  <si>
+    <t>instruction_cheat</t>
+  </si>
+  <si>
+    <t>Press this if you want to skip this level.</t>
   </si>
 </sst>
 </file>
@@ -1559,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D198"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,603 +2118,597 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>198</v>
+        <v>398</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>399</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>366</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>367</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B66" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>368</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>382</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>201</v>
+        <v>400</v>
       </c>
       <c r="B68" t="s">
-        <v>202</v>
+        <v>401</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>363</v>
+        <v>200</v>
       </c>
       <c r="B69" t="s">
-        <v>364</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>365</v>
+        <v>201</v>
       </c>
       <c r="B70" t="s">
-        <v>384</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>363</v>
       </c>
       <c r="B71" t="s">
-        <v>245</v>
+        <v>364</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>365</v>
       </c>
       <c r="B72" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
-        <v>356</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
-        <v>223</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>217</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>233</v>
+        <v>215</v>
+      </c>
+      <c r="B75" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>218</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>397</v>
+        <v>216</v>
+      </c>
+      <c r="B76" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>219</v>
-      </c>
-      <c r="B77" t="s">
-        <v>220</v>
+        <v>217</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>375</v>
-      </c>
-      <c r="B78" t="s">
-        <v>376</v>
+        <v>218</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>377</v>
+        <v>219</v>
       </c>
       <c r="B79" t="s">
-        <v>379</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B80" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>224</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>227</v>
+        <v>377</v>
+      </c>
+      <c r="B81" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>225</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>228</v>
+        <v>378</v>
+      </c>
+      <c r="B82" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>226</v>
-      </c>
-      <c r="B83" t="s">
-        <v>358</v>
+        <v>224</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>383</v>
-      </c>
-      <c r="B84" t="s">
-        <v>381</v>
+        <v>225</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B85" t="s">
-        <v>230</v>
+        <v>358</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>231</v>
+        <v>383</v>
       </c>
       <c r="B86" t="s">
-        <v>232</v>
+        <v>381</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>238</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>315</v>
+        <v>231</v>
+      </c>
+      <c r="B88" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>240</v>
-      </c>
-      <c r="B90" t="s">
-        <v>243</v>
+        <v>238</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B91" t="s">
-        <v>357</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>242</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>359</v>
+        <v>240</v>
+      </c>
+      <c r="B92" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B93" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>250</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>385</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>388</v>
+        <v>248</v>
+      </c>
+      <c r="B95" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>251</v>
-      </c>
-      <c r="B96" t="s">
-        <v>386</v>
+        <v>249</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>252</v>
+        <v>385</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B98" t="s">
-        <v>258</v>
+        <v>386</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>259</v>
+        <v>387</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>261</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>263</v>
+        <v>253</v>
+      </c>
+      <c r="B100" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>316</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>265</v>
-      </c>
-      <c r="B103" t="s">
-        <v>317</v>
+        <v>262</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B105" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>389</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>390</v>
+        <v>269</v>
+      </c>
+      <c r="B107" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>391</v>
+        <v>270</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>392</v>
+        <v>277</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>271</v>
-      </c>
-      <c r="B110" t="s">
-        <v>276</v>
+        <v>391</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>272</v>
+        <v>393</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>274</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>273</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
+      </c>
+      <c r="B112" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>306</v>
+        <v>273</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C116">
-        <v>5</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>279</v>
+        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>285</v>
+        <v>311</v>
+      </c>
+      <c r="C118">
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>203</v>
-      </c>
-      <c r="B121" t="s">
-        <v>204</v>
+        <v>280</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>205</v>
-      </c>
-      <c r="B122" t="s">
-        <v>206</v>
+        <v>282</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>286</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>287</v>
+        <v>203</v>
+      </c>
+      <c r="B123" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>303</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>291</v>
+        <v>205</v>
+      </c>
+      <c r="B124" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>221</v>
-      </c>
-      <c r="B128" t="s">
-        <v>222</v>
+        <v>292</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>254</v>
-      </c>
-      <c r="B129" t="s">
-        <v>257</v>
+        <v>293</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="B130" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>395</v>
+        <v>254</v>
       </c>
       <c r="B131" t="s">
-        <v>396</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>212</v>
+        <v>255</v>
       </c>
       <c r="B132" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>208</v>
+        <v>395</v>
       </c>
       <c r="B133" t="s">
-        <v>209</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B134" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>208</v>
       </c>
       <c r="B135" t="s">
-        <v>11</v>
-      </c>
-      <c r="C135">
-        <v>1</v>
+        <v>209</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>12</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C136">
-        <v>5</v>
+        <v>210</v>
+      </c>
+      <c r="B136" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -2710,10 +2716,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>14</v>
-      </c>
-      <c r="B138" t="s">
-        <v>327</v>
+        <v>12</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C138">
         <v>5</v>
@@ -2721,10 +2727,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="B139" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -2732,10 +2738,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="B140" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C140">
         <v>5</v>
@@ -2743,10 +2749,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B141" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -2754,10 +2760,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B142" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C142">
         <v>5</v>
@@ -2765,10 +2771,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B143" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -2776,10 +2782,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B144" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C144">
         <v>5</v>
@@ -2787,10 +2793,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B145" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -2798,10 +2804,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B146" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C146">
         <v>5</v>
@@ -2809,10 +2815,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B147" t="s">
-        <v>332</v>
+        <v>118</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -2820,10 +2826,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="B148" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C148">
         <v>5</v>
@@ -2831,10 +2837,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B149" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -2842,10 +2848,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>77</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>334</v>
+        <v>75</v>
+      </c>
+      <c r="B150" t="s">
+        <v>333</v>
       </c>
       <c r="C150">
         <v>5</v>
@@ -2853,10 +2859,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B151" t="s">
-        <v>16</v>
+        <v>319</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -2864,10 +2870,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>17</v>
-      </c>
-      <c r="B152" t="s">
-        <v>335</v>
+        <v>77</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="C152">
         <v>5</v>
@@ -2875,10 +2881,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B153" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -2886,10 +2892,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -2897,10 +2903,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B155" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -2908,10 +2914,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -2919,10 +2925,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B157" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -2930,10 +2936,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B158" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="C158">
         <v>5</v>
@@ -2941,10 +2947,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B159" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -2952,10 +2958,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B160" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="C160">
         <v>5</v>
@@ -2963,10 +2969,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B161" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C161">
         <v>1</v>
@@ -2974,10 +2980,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B162" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C162">
         <v>5</v>
@@ -2985,10 +2991,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B163" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -2996,10 +3002,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>41</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>339</v>
+        <v>38</v>
+      </c>
+      <c r="B164" t="s">
+        <v>338</v>
       </c>
       <c r="C164">
         <v>5</v>
@@ -3007,10 +3013,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B165" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -3018,10 +3024,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>44</v>
-      </c>
-      <c r="B166" t="s">
-        <v>360</v>
+        <v>41</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="C166">
         <v>5</v>
@@ -3029,10 +3035,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="B167" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C167">
         <v>1</v>
@@ -3040,10 +3046,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B168" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="C168">
         <v>5</v>
@@ -3051,10 +3057,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B169" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -3062,10 +3068,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>47</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>341</v>
+        <v>80</v>
+      </c>
+      <c r="B170" t="s">
+        <v>340</v>
       </c>
       <c r="C170">
         <v>5</v>
@@ -3073,10 +3079,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B171" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -3084,10 +3090,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>50</v>
-      </c>
-      <c r="B172" t="s">
-        <v>321</v>
+        <v>47</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="C172">
         <v>5</v>
@@ -3095,10 +3101,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B173" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -3106,10 +3112,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>53</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>343</v>
+        <v>50</v>
+      </c>
+      <c r="B174" t="s">
+        <v>321</v>
       </c>
       <c r="C174">
         <v>5</v>
@@ -3117,10 +3123,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B175" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C175">
         <v>1</v>
@@ -3128,10 +3134,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C176">
         <v>5</v>
@@ -3139,10 +3145,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B177" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3150,10 +3156,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>59</v>
-      </c>
-      <c r="B178" t="s">
-        <v>344</v>
+        <v>56</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>342</v>
       </c>
       <c r="C178">
         <v>5</v>
@@ -3161,10 +3167,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B179" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C179">
         <v>1</v>
@@ -3172,10 +3178,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>62</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>345</v>
+        <v>59</v>
+      </c>
+      <c r="B180" t="s">
+        <v>344</v>
       </c>
       <c r="C180">
         <v>5</v>
@@ -3183,10 +3189,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B181" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -3194,10 +3200,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>83</v>
-      </c>
-      <c r="B182" t="s">
-        <v>346</v>
+        <v>62</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="C182">
         <v>5</v>
@@ -3205,21 +3211,21 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B183" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C183">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>86</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>347</v>
+        <v>83</v>
+      </c>
+      <c r="B184" t="s">
+        <v>346</v>
       </c>
       <c r="C184">
         <v>5</v>
@@ -3227,21 +3233,21 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C185">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>89</v>
-      </c>
-      <c r="B186" t="s">
-        <v>323</v>
+        <v>86</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="C186">
         <v>5</v>
@@ -3249,10 +3255,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B187" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -3260,10 +3266,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B188" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C188">
         <v>5</v>
@@ -3271,21 +3277,21 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B189" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C189">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B190" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="C190">
         <v>5</v>
@@ -3293,21 +3299,21 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B191" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C191">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>98</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>350</v>
+        <v>95</v>
+      </c>
+      <c r="B192" t="s">
+        <v>348</v>
       </c>
       <c r="C192">
         <v>5</v>
@@ -3315,10 +3321,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B193" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C193">
         <v>1</v>
@@ -3326,10 +3332,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>101</v>
-      </c>
-      <c r="B194" t="s">
-        <v>325</v>
+        <v>98</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="C194">
         <v>5</v>
@@ -3337,10 +3343,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B195" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C195">
         <v>1</v>
@@ -3348,10 +3354,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>104</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>351</v>
+        <v>101</v>
+      </c>
+      <c r="B196" t="s">
+        <v>325</v>
       </c>
       <c r="C196">
         <v>5</v>
@@ -3359,10 +3365,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B197" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C197">
         <v>1</v>
@@ -3370,12 +3376,34 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>104</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="C198">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>105</v>
+      </c>
+      <c r="B199" t="s">
+        <v>106</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>107</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C198">
+      <c r="C200">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove rock/mineral/organic add/remove (unlimited supply), fix fade in/out sprite shapes, some other minor crap
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D42B8-A11A-4C15-96B3-D951501B74B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13EF489-77BE-4B6D-86DD-580B9B3F88CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
   <si>
     <t>Key</t>
   </si>
@@ -1226,6 +1226,12 @@
   </si>
   <si>
     <t>Press this if you want to skip this level.</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -1571,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,1675 +1741,1683 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>402</v>
       </c>
       <c r="B18" t="s">
-        <v>149</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B22" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>247</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>246</v>
       </c>
       <c r="B26" t="s">
-        <v>155</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>178</v>
       </c>
       <c r="C30">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>297</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>298</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>299</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>120</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>122</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>295</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>124</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>158</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>159</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>362</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>164</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>162</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>313</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>369</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>371</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>372</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>373</v>
-      </c>
-      <c r="B48" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>373</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>188</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>353</v>
+        <v>185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>189</v>
-      </c>
-      <c r="B59" t="s">
-        <v>354</v>
+        <v>188</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B60" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
+        <v>352</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B63" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>398</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s">
-        <v>399</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>198</v>
+        <v>398</v>
       </c>
       <c r="B65" t="s">
-        <v>199</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>366</v>
+        <v>198</v>
       </c>
       <c r="B66" t="s">
-        <v>367</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B67" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="B68" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>401</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>363</v>
+        <v>201</v>
       </c>
       <c r="B71" t="s">
-        <v>364</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B72" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>365</v>
       </c>
       <c r="B73" t="s">
-        <v>245</v>
+        <v>384</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>355</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>356</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>217</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
+      </c>
+      <c r="B77" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>397</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>219</v>
-      </c>
-      <c r="B79" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>375</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s">
-        <v>376</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B81" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B82" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>224</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>227</v>
+        <v>378</v>
+      </c>
+      <c r="B83" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>226</v>
-      </c>
-      <c r="B85" t="s">
-        <v>358</v>
+        <v>225</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>383</v>
+        <v>226</v>
       </c>
       <c r="B86" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>383</v>
       </c>
       <c r="B87" t="s">
-        <v>230</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>238</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>315</v>
+        <v>236</v>
+      </c>
+      <c r="B90" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>239</v>
-      </c>
-      <c r="B91" t="s">
-        <v>244</v>
+        <v>238</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B92" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B93" t="s">
-        <v>357</v>
+        <v>243</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>242</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>359</v>
+        <v>241</v>
+      </c>
+      <c r="B94" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>248</v>
-      </c>
-      <c r="B95" t="s">
-        <v>318</v>
+        <v>242</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>249</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="B96" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>385</v>
+        <v>249</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>388</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>251</v>
-      </c>
-      <c r="B98" t="s">
-        <v>386</v>
+        <v>385</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>252</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>387</v>
+        <v>251</v>
+      </c>
+      <c r="B99" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>253</v>
-      </c>
-      <c r="B100" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>260</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
+      </c>
+      <c r="B101" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>316</v>
+        <v>263</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>265</v>
-      </c>
-      <c r="B105" t="s">
-        <v>317</v>
+        <v>264</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>266</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
+      </c>
+      <c r="B106" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>269</v>
-      </c>
-      <c r="B107" t="s">
-        <v>312</v>
+        <v>266</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>270</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>277</v>
+        <v>269</v>
+      </c>
+      <c r="B108" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>389</v>
+        <v>270</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>390</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>271</v>
-      </c>
-      <c r="B112" t="s">
-        <v>276</v>
+        <v>393</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>272</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B113" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C118">
-        <v>5</v>
+        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>278</v>
+        <v>310</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>279</v>
+        <v>311</v>
+      </c>
+      <c r="C119">
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>203</v>
-      </c>
-      <c r="B123" t="s">
-        <v>204</v>
+        <v>282</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B124" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>286</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>287</v>
+        <v>205</v>
+      </c>
+      <c r="B125" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>221</v>
-      </c>
-      <c r="B130" t="s">
-        <v>222</v>
+        <v>293</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>254</v>
+        <v>221</v>
       </c>
       <c r="B131" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B132" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>395</v>
+        <v>255</v>
       </c>
       <c r="B133" t="s">
-        <v>396</v>
+        <v>256</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>212</v>
+        <v>395</v>
       </c>
       <c r="B134" t="s">
-        <v>207</v>
+        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B135" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B136" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="B137" t="s">
-        <v>11</v>
-      </c>
-      <c r="C137">
-        <v>1</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>12</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>326</v>
+        <v>10</v>
+      </c>
+      <c r="B138" t="s">
+        <v>11</v>
       </c>
       <c r="C138">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>9</v>
-      </c>
-      <c r="B139" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="C139">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B140" t="s">
-        <v>327</v>
+        <v>13</v>
       </c>
       <c r="C140">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>109</v>
+        <v>327</v>
       </c>
       <c r="C141">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B142" t="s">
-        <v>328</v>
+        <v>109</v>
       </c>
       <c r="C142">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>112</v>
+        <v>328</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B144" t="s">
-        <v>329</v>
+        <v>112</v>
       </c>
       <c r="C144">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B145" t="s">
-        <v>115</v>
+        <v>329</v>
       </c>
       <c r="C145">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B146" t="s">
-        <v>330</v>
+        <v>115</v>
       </c>
       <c r="C146">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B147" t="s">
-        <v>118</v>
+        <v>330</v>
       </c>
       <c r="C147">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B148" t="s">
-        <v>331</v>
+        <v>118</v>
       </c>
       <c r="C148">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B149" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B150" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C150">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B151" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>77</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>334</v>
+        <v>76</v>
+      </c>
+      <c r="B152" t="s">
+        <v>319</v>
       </c>
       <c r="C152">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>15</v>
-      </c>
-      <c r="B153" t="s">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>334</v>
       </c>
       <c r="C153">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B154" t="s">
-        <v>335</v>
+        <v>16</v>
       </c>
       <c r="C154">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>19</v>
+        <v>335</v>
       </c>
       <c r="C155">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B156" t="s">
-        <v>320</v>
+        <v>19</v>
       </c>
       <c r="C156">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>22</v>
+        <v>320</v>
       </c>
       <c r="C157">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B158" t="s">
-        <v>336</v>
+        <v>22</v>
       </c>
       <c r="C158">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B159" t="s">
-        <v>25</v>
+        <v>336</v>
       </c>
       <c r="C159">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B160" t="s">
-        <v>324</v>
+        <v>25</v>
       </c>
       <c r="C160">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B161" t="s">
-        <v>34</v>
+        <v>324</v>
       </c>
       <c r="C161">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B162" t="s">
-        <v>337</v>
+        <v>34</v>
       </c>
       <c r="C162">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B163" t="s">
-        <v>37</v>
+        <v>337</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B164" t="s">
-        <v>338</v>
+        <v>37</v>
       </c>
       <c r="C164">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B165" t="s">
-        <v>39</v>
+        <v>338</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>41</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>339</v>
+        <v>40</v>
+      </c>
+      <c r="B166" t="s">
+        <v>39</v>
       </c>
       <c r="C166">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>42</v>
-      </c>
-      <c r="B167" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>339</v>
       </c>
       <c r="C167">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B168" t="s">
-        <v>360</v>
+        <v>43</v>
       </c>
       <c r="C168">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="B169" t="s">
-        <v>79</v>
+        <v>360</v>
       </c>
       <c r="C169">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B170" t="s">
-        <v>340</v>
+        <v>79</v>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B171" t="s">
-        <v>46</v>
+        <v>340</v>
       </c>
       <c r="C171">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>47</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>341</v>
+        <v>45</v>
+      </c>
+      <c r="B172" t="s">
+        <v>46</v>
       </c>
       <c r="C172">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>48</v>
-      </c>
-      <c r="B173" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="C173">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B174" t="s">
-        <v>321</v>
+        <v>49</v>
       </c>
       <c r="C174">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B175" t="s">
-        <v>52</v>
+        <v>321</v>
       </c>
       <c r="C175">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>53</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>343</v>
+        <v>51</v>
+      </c>
+      <c r="B176" t="s">
+        <v>52</v>
       </c>
       <c r="C176">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>54</v>
-      </c>
-      <c r="B177" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="C177">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>56</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>342</v>
+        <v>54</v>
+      </c>
+      <c r="B178" t="s">
+        <v>55</v>
       </c>
       <c r="C178">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>57</v>
-      </c>
-      <c r="B179" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>342</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B180" t="s">
-        <v>344</v>
+        <v>58</v>
       </c>
       <c r="C180">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B181" t="s">
-        <v>61</v>
+        <v>344</v>
       </c>
       <c r="C181">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>62</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>345</v>
+        <v>60</v>
+      </c>
+      <c r="B182" t="s">
+        <v>61</v>
       </c>
       <c r="C182">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>81</v>
-      </c>
-      <c r="B183" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="C183">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B184" t="s">
-        <v>346</v>
+        <v>82</v>
       </c>
       <c r="C184">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B185" t="s">
-        <v>85</v>
+        <v>346</v>
       </c>
       <c r="C185">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>86</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>347</v>
+        <v>84</v>
+      </c>
+      <c r="B186" t="s">
+        <v>85</v>
       </c>
       <c r="C186">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>87</v>
-      </c>
-      <c r="B187" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="C187">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B188" t="s">
-        <v>323</v>
+        <v>88</v>
       </c>
       <c r="C188">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B189" t="s">
-        <v>91</v>
+        <v>323</v>
       </c>
       <c r="C189">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B190" t="s">
-        <v>322</v>
+        <v>91</v>
       </c>
       <c r="C190">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B191" t="s">
-        <v>94</v>
+        <v>322</v>
       </c>
       <c r="C191">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B192" t="s">
-        <v>348</v>
+        <v>94</v>
       </c>
       <c r="C192">
-        <v>5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B193" t="s">
-        <v>97</v>
+        <v>348</v>
       </c>
       <c r="C193">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>98</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>350</v>
+        <v>96</v>
+      </c>
+      <c r="B194" t="s">
+        <v>97</v>
       </c>
       <c r="C194">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>99</v>
-      </c>
-      <c r="B195" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>350</v>
       </c>
       <c r="C195">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B196" t="s">
-        <v>325</v>
+        <v>100</v>
       </c>
       <c r="C196">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B197" t="s">
-        <v>103</v>
+        <v>325</v>
       </c>
       <c r="C197">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>104</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>351</v>
+        <v>102</v>
+      </c>
+      <c r="B198" t="s">
+        <v>103</v>
       </c>
       <c r="C198">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>105</v>
-      </c>
-      <c r="B199" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>351</v>
       </c>
       <c r="C199">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>105</v>
+      </c>
+      <c r="B200" t="s">
+        <v>106</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>107</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B201" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="C200">
+      <c r="C201">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed hold-press to just click, remove locked rock display
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13EF489-77BE-4B6D-86DD-580B9B3F88CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD955F1-8D5F-412C-8501-A8705FC7F1F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,9 +691,6 @@
     <t>We require magma to form igneous rocks. Head over to the Magma Chamber.</t>
   </si>
   <si>
-    <t>Go ahead and process the minerals by holding the Spacebar (you can also click and hold the icon).</t>
-  </si>
-  <si>
     <t>intro_intrusive_igneous_1</t>
   </si>
   <si>
@@ -1232,6 +1229,9 @@
   </si>
   <si>
     <t>SKIP</t>
+  </si>
+  <si>
+    <t>Go ahead and process the minerals by pressing the Spacebar (you can also click the icon).</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,10 +1741,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" t="s">
         <v>402</v>
-      </c>
-      <c r="B18" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,10 +1805,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
         <v>246</v>
-      </c>
-      <c r="B26" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1884,26 +1884,26 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1924,10 +1924,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" t="s">
         <v>295</v>
-      </c>
-      <c r="B39" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1956,10 +1956,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B43" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,34 +1980,34 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>312</v>
+      </c>
+      <c r="B46" t="s">
         <v>313</v>
-      </c>
-      <c r="B46" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>368</v>
+      </c>
+      <c r="B47" t="s">
         <v>369</v>
-      </c>
-      <c r="B47" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>370</v>
+      </c>
+      <c r="B48" t="s">
         <v>371</v>
-      </c>
-      <c r="B48" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B49" t="s">
         <v>373</v>
-      </c>
-      <c r="B49" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>188</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
         <v>189</v>
       </c>
       <c r="B60" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>190</v>
       </c>
       <c r="B61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2132,10 +2132,10 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>397</v>
+      </c>
+      <c r="B65" t="s">
         <v>398</v>
-      </c>
-      <c r="B65" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2148,26 +2148,26 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>365</v>
+      </c>
+      <c r="B67" t="s">
         <v>366</v>
-      </c>
-      <c r="B67" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B68" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" t="s">
         <v>400</v>
-      </c>
-      <c r="B69" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
         <v>200</v>
       </c>
       <c r="B70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2188,18 +2188,18 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>362</v>
+      </c>
+      <c r="B72" t="s">
         <v>363</v>
-      </c>
-      <c r="B72" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B73" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>213</v>
       </c>
       <c r="B74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,7 +2215,7 @@
         <v>214</v>
       </c>
       <c r="B75" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
         <v>215</v>
       </c>
       <c r="B76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2231,7 +2231,7 @@
         <v>216</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>403</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2239,7 +2239,7 @@
         <v>217</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>218</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2260,314 +2260,314 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>374</v>
+      </c>
+      <c r="B81" t="s">
         <v>375</v>
-      </c>
-      <c r="B81" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B82" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B83" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B87" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" t="s">
         <v>229</v>
-      </c>
-      <c r="B88" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>230</v>
+      </c>
+      <c r="B89" t="s">
         <v>231</v>
-      </c>
-      <c r="B89" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>235</v>
+      </c>
+      <c r="B90" t="s">
         <v>236</v>
-      </c>
-      <c r="B90" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B92" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B94" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B96" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B101" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B106" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B108" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>388</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>390</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B113" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>303</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>305</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>307</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="C119">
         <v>5</v>
@@ -2575,34 +2575,34 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>277</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>283</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>279</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>281</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -2623,42 +2623,42 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>285</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>287</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,26 +2671,26 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B132" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" t="s">
         <v>255</v>
-      </c>
-      <c r="B133" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>394</v>
+      </c>
+      <c r="B134" t="s">
         <v>395</v>
-      </c>
-      <c r="B134" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -2733,7 +2733,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C139">
         <v>5</v>
@@ -2755,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="B141" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C141">
         <v>5</v>
@@ -2777,7 +2777,7 @@
         <v>110</v>
       </c>
       <c r="B143" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C143">
         <v>5</v>
@@ -2799,7 +2799,7 @@
         <v>113</v>
       </c>
       <c r="B145" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C145">
         <v>5</v>
@@ -2821,7 +2821,7 @@
         <v>116</v>
       </c>
       <c r="B147" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C147">
         <v>5</v>
@@ -2843,7 +2843,7 @@
         <v>119</v>
       </c>
       <c r="B149" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -2854,7 +2854,7 @@
         <v>74</v>
       </c>
       <c r="B150" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -2865,7 +2865,7 @@
         <v>75</v>
       </c>
       <c r="B151" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C151">
         <v>5</v>
@@ -2876,7 +2876,7 @@
         <v>76</v>
       </c>
       <c r="B152" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -2887,7 +2887,7 @@
         <v>77</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C153">
         <v>5</v>
@@ -2909,7 +2909,7 @@
         <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C155">
         <v>5</v>
@@ -2931,7 +2931,7 @@
         <v>20</v>
       </c>
       <c r="B157" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C157">
         <v>5</v>
@@ -2953,7 +2953,7 @@
         <v>23</v>
       </c>
       <c r="B159" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C159">
         <v>5</v>
@@ -2975,7 +2975,7 @@
         <v>26</v>
       </c>
       <c r="B161" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C161">
         <v>5</v>
@@ -2997,7 +2997,7 @@
         <v>35</v>
       </c>
       <c r="B163" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C163">
         <v>5</v>
@@ -3019,7 +3019,7 @@
         <v>38</v>
       </c>
       <c r="B165" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C165">
         <v>5</v>
@@ -3041,7 +3041,7 @@
         <v>41</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C167">
         <v>5</v>
@@ -3063,7 +3063,7 @@
         <v>44</v>
       </c>
       <c r="B169" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C169">
         <v>5</v>
@@ -3085,7 +3085,7 @@
         <v>80</v>
       </c>
       <c r="B171" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C171">
         <v>5</v>
@@ -3107,7 +3107,7 @@
         <v>47</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C173">
         <v>5</v>
@@ -3129,7 +3129,7 @@
         <v>50</v>
       </c>
       <c r="B175" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C175">
         <v>5</v>
@@ -3151,7 +3151,7 @@
         <v>53</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C177">
         <v>5</v>
@@ -3173,7 +3173,7 @@
         <v>56</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C179">
         <v>5</v>
@@ -3195,7 +3195,7 @@
         <v>59</v>
       </c>
       <c r="B181" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C181">
         <v>5</v>
@@ -3217,7 +3217,7 @@
         <v>62</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C183">
         <v>5</v>
@@ -3239,7 +3239,7 @@
         <v>83</v>
       </c>
       <c r="B185" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C185">
         <v>5</v>
@@ -3261,7 +3261,7 @@
         <v>86</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C187">
         <v>5</v>
@@ -3283,7 +3283,7 @@
         <v>89</v>
       </c>
       <c r="B189" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C189">
         <v>5</v>
@@ -3305,7 +3305,7 @@
         <v>92</v>
       </c>
       <c r="B191" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C191">
         <v>5</v>
@@ -3327,7 +3327,7 @@
         <v>95</v>
       </c>
       <c r="B193" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C193">
         <v>5</v>
@@ -3349,7 +3349,7 @@
         <v>98</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C195">
         <v>5</v>
@@ -3371,7 +3371,7 @@
         <v>101</v>
       </c>
       <c r="B197" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C197">
         <v>5</v>
@@ -3393,7 +3393,7 @@
         <v>104</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C199">
         <v>5</v>
@@ -3415,7 +3415,7 @@
         <v>107</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C201">
         <v>5</v>

</xml_diff>

<commit_message>
added spanish language, upgrade to latest unity 2019 version, upgrade lol sdk
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD955F1-8D5F-412C-8501-A8705FC7F1F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DCACA6-DCC4-495D-9841-4602632A6BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
+    <sheet name="es" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="600">
   <si>
     <t>Key</t>
   </si>
@@ -1232,6 +1233,594 @@
   </si>
   <si>
     <t>Go ahead and process the minerals by pressing the Spacebar (you can also click the icon).</t>
+  </si>
+  <si>
+    <t>¡Bienvenido!</t>
+  </si>
+  <si>
+    <t>Súper Gnomático Ciclismo de Roca</t>
+  </si>
+  <si>
+    <t>CRÉDITOS</t>
+  </si>
+  <si>
+    <t>Escrito por:\nDavid Dionisio\nMúsica de:\nKevin Macleod</t>
+  </si>
+  <si>
+    <t>COMENZAR</t>
+  </si>
+  <si>
+    <t>OPCIONES</t>
+  </si>
+  <si>
+    <t>MÚSICA</t>
+  </si>
+  <si>
+    <t>SONIDO</t>
+  </si>
+  <si>
+    <t>DISCURSO</t>
+  </si>
+  <si>
+    <t>REINICIAR</t>
+  </si>
+  <si>
+    <t>CERRAR</t>
+  </si>
+  <si>
+    <t>APAGADO</t>
+  </si>
+  <si>
+    <t>ENCENDIDO</t>
+  </si>
+  <si>
+    <t>¿Estás seguro de que quieres reiniciar el nivel?</t>
+  </si>
+  <si>
+    <t>SÍ</t>
+  </si>
+  <si>
+    <t>SALTAR</t>
+  </si>
+  <si>
+    <t>Método Selecto</t>
+  </si>
+  <si>
+    <t>Seleccionar Origen</t>
+  </si>
+  <si>
+    <t>Intrusiva</t>
+  </si>
+  <si>
+    <t>Extrusivo</t>
+  </si>
+  <si>
+    <t>Roca</t>
+  </si>
+  <si>
+    <t>Rocas</t>
+  </si>
+  <si>
+    <t>Orgánicos</t>
+  </si>
+  <si>
+    <t>Sedimentos</t>
+  </si>
+  <si>
+    <t>Para atras</t>
+  </si>
+  <si>
+    <t>PROCEDER</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>COLECCIONES</t>
+  </si>
+  <si>
+    <t>Ígneo</t>
+  </si>
+  <si>
+    <t>Sedimentario</t>
+  </si>
+  <si>
+    <t>Metamórfico</t>
+  </si>
+  <si>
+    <t>Piedra ígnea</t>
+  </si>
+  <si>
+    <t>Roca sedimentaria</t>
+  </si>
+  <si>
+    <t>Piedra metamórfico</t>
+  </si>
+  <si>
+    <t>* NUEVO *</t>
+  </si>
+  <si>
+    <t>Minerales</t>
+  </si>
+  <si>
+    <t>Refrigeración...</t>
+  </si>
+  <si>
+    <t>PARAR</t>
+  </si>
+  <si>
+    <t>EL CICLO DE ROCAS</t>
+  </si>
+  <si>
+    <t>RESULTADO DE PIEDRAS</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>COMPLETAR</t>
+  </si>
+  <si>
+    <t>ENTRAR EN CÁMARA DE MAGMA</t>
+  </si>
+  <si>
+    <t>ENTRAR EN EL REFRIGERADOR DE MAGMA</t>
+  </si>
+  <si>
+    <t>ENTRAR EN FOSO SEDIMENTARIO</t>
+  </si>
+  <si>
+    <t>EROSIONAR</t>
+  </si>
+  <si>
+    <t>Tamaño de grano</t>
+  </si>
+  <si>
+    <t>Adoquines</t>
+  </si>
+  <si>
+    <t>Arena</t>
+  </si>
+  <si>
+    <t>Limo</t>
+  </si>
+  <si>
+    <t>Arcilla</t>
+  </si>
+  <si>
+    <t>Cristales finos a gruesos.</t>
+  </si>
+  <si>
+    <t>Microscópica a muy gruesa.</t>
+  </si>
+  <si>
+    <t>Bienvenido al Ciclador de Rocas Supergnomático!</t>
+  </si>
+  <si>
+    <t>Las piedras están formadas por minerales que se formaron y unieron.</t>
+  </si>
+  <si>
+    <t>En función de cómo se forma, cada roca se clasifica en uno de estos grupos: ígnea, sedimentaria, metamórfica.</t>
+  </si>
+  <si>
+    <t>Más adelante investigaremos más detalles.</t>
+  </si>
+  <si>
+    <t>Por ahora, sigamos adelante y recojamos algunos minerales.</t>
+  </si>
+  <si>
+    <t>Presiona las teclas de flecha izquierda o derecha para mover al gnomo.</t>
+  </si>
+  <si>
+    <t>Pulse la barra espaciadora para entrar.</t>
+  </si>
+  <si>
+    <t>Presiona la barra espaciadora para enviarla.</t>
+  </si>
+  <si>
+    <t>Presiona la barra espaciadora o la flecha arriba para saltar.</t>
+  </si>
+  <si>
+    <t>Pulsa este botón para salir y continuar.</t>
+  </si>
+  <si>
+    <t>¡Ahora tienes los tipos de piedra necesarios! Pulsa este botón para salir y continuar.</t>
+  </si>
+  <si>
+    <t>Presiona esta tecla si quieres saltarte este nivel.</t>
+  </si>
+  <si>
+    <t>Ahora que tienes algunos minerales, es hora de derretirlos en magma.</t>
+  </si>
+  <si>
+    <t>Dirígete a la Cámara de Magma para hacerlo.</t>
+  </si>
+  <si>
+    <t>En esta parte del ciclo rocoso, veremos que las piedras se derriten hasta el magma.</t>
+  </si>
+  <si>
+    <t>Como puedes ver, todas las piedras se derriten hasta convertirlas en magma.</t>
+  </si>
+  <si>
+    <t>En la Tierra, las piedras se empujan continuamente hacia arriba o hacia abajo debido a fuerzas poderosas como un terremoto.</t>
+  </si>
+  <si>
+    <t>Cuando una piedra es empujada lo suficientemente profundamente en la Tierra, las temperaturas pueden alcanzar su punto de fusión y derretirla. Cuando la piedra se derrita, se convertirá en magma.</t>
+  </si>
+  <si>
+    <t>Aquí, en la Cámara Magma, simularemos el proceso de derretir piedras en magma.</t>
+  </si>
+  <si>
+    <t>Continúa y procesa los minerales presionando la barra espaciadora (también puedes hacer clic en el icono).</t>
+  </si>
+  <si>
+    <t>Ahora que tenemos magma disponible, ¡es hora de formar unas rocas!</t>
+  </si>
+  <si>
+    <t>Si observas la barra en la parte superior, verás que necesitamos formar al menos tres tipos diferentes de rocas ígneas.</t>
+  </si>
+  <si>
+    <t>Para formar piedras ígneas, dirígete al Enfriador de Magma.</t>
+  </si>
+  <si>
+    <t>Para este ciclo de piedras, veremos que el magma se enfría y se solidifica hasta convertirnos en una piedra.</t>
+  </si>
+  <si>
+    <t>Cuando el magma se empuja hacia arriba debido al flujo de energía dentro de la Tierra, eventualmente se enfriará y se cristalizará en varios minerales.</t>
+  </si>
+  <si>
+    <t>Durante la cristalización, varios minerales se formarán y se unirán entre sí, convirtiéndose en una piedra ígnea.</t>
+  </si>
+  <si>
+    <t>Existen dos formas de formarse piedras ígneas: intrusivas o extrusivas.</t>
+  </si>
+  <si>
+    <t>Por ahora, formaremos piedras ígneas intrusivas.</t>
+  </si>
+  <si>
+    <t>Las piedras ígneas intrusivas se forman cuando el magma se enfría por debajo de la superficie terrestre.</t>
+  </si>
+  <si>
+    <t>Pulse la barra espaciadora o haga clic en este botón para continuar.</t>
+  </si>
+  <si>
+    <t>Ahora que has formado las piedras necesarias, es hora de dejarlas caer.</t>
+  </si>
+  <si>
+    <t>¡Dirígete a la estrella indicada y envía las piedras!</t>
+  </si>
+  <si>
+    <t>¡Excelente trabajo! Ahora que se han presentado las piedras, podemos reunir más minerales para formar nuevas piedras.</t>
+  </si>
+  <si>
+    <t>Al igual que antes, necesitamos formar tres tipos diferentes de piedras ígneas.</t>
+  </si>
+  <si>
+    <t>Recuerda derretir los minerales en la cámara de magma y luego formar las rocas en el refrigerador de magma.</t>
+  </si>
+  <si>
+    <t>Esta vez, vamos a formar piedras ígneas extrusivas.</t>
+  </si>
+  <si>
+    <t>Estas piedras se forman cuando el magma se enfría por encima de la superficie terrestre. Por ejemplo: después de que estalla un volcán.</t>
+  </si>
+  <si>
+    <t>Como estas piedras se enfrían más rápido, no forman tantos cristales como piedras ígneas intrusivas.</t>
+  </si>
+  <si>
+    <t>Para que se formen piedras sedimentarias, primero debemos tener piedras disponibles para descomponerse en sedimentos.</t>
+  </si>
+  <si>
+    <t>Sigue adelante y crea piedras ígneas antes de dirigirte al pozo sedimentario.</t>
+  </si>
+  <si>
+    <t>Para este ciclo rocoso, veremos cómo las rocas se dividen en sedimentos y luego se forman una roca sedimentaria.</t>
+  </si>
+  <si>
+    <t>Los sedimentos proceden de cualquier tipo de piedras, o de ciertos materiales orgánicos que se han desglosado por la intemperie y la erosión.</t>
+  </si>
+  <si>
+    <t>Después de un largo período de tiempo, los sedimentos que se han acumulado en un área se compactarán y se cementarán para formar piedras sedimentarias.</t>
+  </si>
+  <si>
+    <t>Aquí, en el pozo sedimentario, simularemos el proceso de descomponer piedras en sedimentos y luego cementarlo para formar una nueva piedra.</t>
+  </si>
+  <si>
+    <t>El resultado de la roca sedimentaria se basará en el tamaño de grano de los sedimentos. Por lo tanto, asegúrate de probar diferentes tamaños.</t>
+  </si>
+  <si>
+    <t>En esta ocasión, haremos piedras sedimentarias con materiales orgánicos.</t>
+  </si>
+  <si>
+    <t>Dirígete directamente al pozo sedimentario.</t>
+  </si>
+  <si>
+    <t>Las piedras sedimentarias se pueden formar a partir de los restos de ciertas formas de vida.</t>
+  </si>
+  <si>
+    <t>Por ejemplo, las plantas y árboles enterrados durante millones de años pueden convertirse en carbón.</t>
+  </si>
+  <si>
+    <t>Si tienes suerte, puedes encontrar uno o dos fósiles de este tipo de piedras.</t>
+  </si>
+  <si>
+    <t>Para nuestro último tipo de piedra: Metamorfa, vamos a necesitar formar otras rocas.</t>
+  </si>
+  <si>
+    <t>Una vez que tengas un montón de rocas disponibles, dirígete al pozo metamórfico.</t>
+  </si>
+  <si>
+    <t>Para este ciclo de piedras, veremos cómo las piedras se transforman en piedra metamórfica.</t>
+  </si>
+  <si>
+    <t>Como puedes ver, todas las piedras finalmente se hunden debajo de la Tierra, formando una piedra diferente.</t>
+  </si>
+  <si>
+    <t>Y por último, hundirse aún más para derretirse en magma, completando el ciclo rocoso.</t>
+  </si>
+  <si>
+    <t>Cuando una piedra está sometida a suficiente calor y/o presión, su forma cambiará drásticamente, transformándose en una piedra completamente diferente.</t>
+  </si>
+  <si>
+    <t>Dependiendo del tipo de piedra que elijas, el resultado será diferente.</t>
+  </si>
+  <si>
+    <t>Intenta transformar una piedra previamente transformada para obtener otro tipo de piedra.</t>
+  </si>
+  <si>
+    <t>¡En hora buena! ¡Has reunido todas las piedras que necesitamos!</t>
+  </si>
+  <si>
+    <t>¡Esto termina El Ciclador de Rocas Supergnomático!</t>
+  </si>
+  <si>
+    <t>Tipos de piedra recolectada: {0} de {1}.</t>
+  </si>
+  <si>
+    <t>¡Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>Expedición</t>
+  </si>
+  <si>
+    <t>Entregar</t>
+  </si>
+  <si>
+    <t>Fosa sedimentaria</t>
+  </si>
+  <si>
+    <t>Fosa metamórfica</t>
+  </si>
+  <si>
+    <t>Cámara de magma</t>
+  </si>
+  <si>
+    <t>Enfriador de Magma</t>
+  </si>
+  <si>
+    <t>Derritiendo</t>
+  </si>
+  <si>
+    <t>Enfriamiento</t>
+  </si>
+  <si>
+    <t>Calor y presión</t>
+  </si>
+  <si>
+    <t>Intemperie y erosión</t>
+  </si>
+  <si>
+    <t>Compactación y cementación</t>
+  </si>
+  <si>
+    <t>Necesitamos magma para formar piedras ígneas. Dirígete a la Cámara de Magma.</t>
+  </si>
+  <si>
+    <t>Necesitamos al menos tres piedras para formar una piedra sedimentaria. Dirígete al Enfriador de Magma para formar algo.</t>
+  </si>
+  <si>
+    <t>Necesitamos rocas para formar rocas metamórficas. Dirígete al Enfriador de Magma o al Pozo Sedimentario para formar algunas.</t>
+  </si>
+  <si>
+    <t>Debe llenar las ranuras de piedra antes de enviarlas.</t>
+  </si>
+  <si>
+    <t>Corteza</t>
+  </si>
+  <si>
+    <t>Manto</t>
+  </si>
+  <si>
+    <t>Tierra</t>
+  </si>
+  <si>
+    <t>Olivino</t>
+  </si>
+  <si>
+    <t>Un mineral que suele ser de color verde. Por lo general, se puede encontrar en rocas ígneas y metamórficas.</t>
+  </si>
+  <si>
+    <t>Cuarzo</t>
+  </si>
+  <si>
+    <t>Mineral que suele ser incoloro o de color claro. Se puede encontrar comúnmente en la superficie de la Tierra.</t>
+  </si>
+  <si>
+    <t>Feldespato</t>
+  </si>
+  <si>
+    <t>Uno de los minerales comunes que se encuentran en la corteza terrestre. La mayoría de las piedras están compuestas por este mineral.</t>
+  </si>
+  <si>
+    <t>Piroxeno</t>
+  </si>
+  <si>
+    <t>Este mineral tiende a estar presente en las lavas volcánicas. Su color suele ser negro, a veces con un toque verde.</t>
+  </si>
+  <si>
+    <t>Anfíbol</t>
+  </si>
+  <si>
+    <t>Este mineral se encuentra principalmente en piedras ígneas y metamórficas. Los anfíboles vienen en una variedad de colores: verde, negro, incoloro, blanco, amarillo, azul o marrón.</t>
+  </si>
+  <si>
+    <t>Biotita</t>
+  </si>
+  <si>
+    <t>Este mineral se encuentra comúnmente en piedras ígneas y metamórficas. Su color suele ser negro, marrón oscuro o verde oscuro.</t>
+  </si>
+  <si>
+    <t>Caracoles marinos</t>
+  </si>
+  <si>
+    <t>Estos materiales son el ingrediente clave para fabricar piedra caliza mediante compactación y cementación.</t>
+  </si>
+  <si>
+    <t>Madera</t>
+  </si>
+  <si>
+    <t>Las plantas muertas y la madera enterradas en las profundidades de la Tierra pueden convertirse lentamente en carbón, un tipo de roca sedimentaria.</t>
+  </si>
+  <si>
+    <t>Peridotita</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de grano grueso y de color oscuro. Por lo general, contiene olivino mineral.</t>
+  </si>
+  <si>
+    <t>Gabro</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de grano grueso. Su color suele ser negro o verde oscuro.</t>
+  </si>
+  <si>
+    <t>Diorita</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de grano grueso conocida por su aspecto de sal y pimienta.</t>
+  </si>
+  <si>
+    <t>Granito</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de color claro con grandes granos visibles. Está compuesto principalmente de cuarzo y feldespato, lo que lo hace duro y resistente.</t>
+  </si>
+  <si>
+    <t>Piedra pómez</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de color claro que se forma durante una erupción volcánica. Tiene una textura porosa.</t>
+  </si>
+  <si>
+    <t>Escoria volcánica</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de color oscuro que se forma durante una erupción volcánica. Su textura está compuesta por cavidades tipo burbuja.</t>
+  </si>
+  <si>
+    <t>Ryolita</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea extrusiva que suele ser de color rosa o gris.</t>
+  </si>
+  <si>
+    <t>Basalto</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea de grano fino que suele ser de color negro. Estos se encuentran comúnmente en el fondo oceánico.</t>
+  </si>
+  <si>
+    <t>Obsidiana</t>
+  </si>
+  <si>
+    <t>Una piedra ígnea que se forma cuando la lava se enfría rápidamente, lo que da como resultado su aspecto vidrioso negro.</t>
+  </si>
+  <si>
+    <t>Brecha</t>
+  </si>
+  <si>
+    <t>Piedra sedimentaria compuesta por grandes fragmentos de forma angular pegados entre sí.</t>
+  </si>
+  <si>
+    <t>Arenisca</t>
+  </si>
+  <si>
+    <t>Piedra sedimentaria compuesta de sedimentos de arena. Su textura es rugosa y natural, con una amplia gama de colores.</t>
+  </si>
+  <si>
+    <t>Esquisto</t>
+  </si>
+  <si>
+    <t>Piedra sedimentaria de grano fino formada a partir de la compactación de sedimentos arcillosos.</t>
+  </si>
+  <si>
+    <t>Limolita</t>
+  </si>
+  <si>
+    <t>Piedra sedimentaria de grano fino formada a partir de la compactación de sedimentos de limo.</t>
+  </si>
+  <si>
+    <t>Carbón bituminoso</t>
+  </si>
+  <si>
+    <t>Carbón blando que se forma a partir de desechos vegetales que se desoxigenan y se entierran profundamente en los sedimentos durante mucho tiempo.</t>
+  </si>
+  <si>
+    <t>Caliza</t>
+  </si>
+  <si>
+    <t>Piedra sedimentaria compuesta principalmente de calcita. Estas calcitas se forman a partir de la acumulación de caracoles y esqueletos compactados juntos.</t>
+  </si>
+  <si>
+    <t>Anfibolita</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica de grano grueso que tiende a formarse a partir de piedras ígneas debido a la alta presión.</t>
+  </si>
+  <si>
+    <t>Carbón antracita</t>
+  </si>
+  <si>
+    <t>Tipo de carbón que ha sufrido calor y presión. Esto da como resultado un aspecto brillante y brillante.</t>
+  </si>
+  <si>
+    <t>Gneis</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica con patrones de rayas. Sus rayas están formadas por capas de piedras preexistentes.</t>
+  </si>
+  <si>
+    <t>Mármol</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica con patrones nublados. Está formado por minerales que se han cristalizado debido al calor y la presión.</t>
+  </si>
+  <si>
+    <t>Metaconglomerato</t>
+  </si>
+  <si>
+    <t>Versión transformada de una piedra de conglomerado, como la brecha, que ha sufrido calor y presión.</t>
+  </si>
+  <si>
+    <t>Filita</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica con una superficie parecida a una lámina que resplandece de su diminuto grano de cristales.</t>
+  </si>
+  <si>
+    <t>Cuarcita</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica hecha de cuarzo. Estos cuarzo suelen proceder de arenisca.</t>
+  </si>
+  <si>
+    <t>Una piedra metamórfica compuesta de cristales platinos formados por arcilla que ha sufrido calor y presión.</t>
+  </si>
+  <si>
+    <t>Pizarra (roca)</t>
+  </si>
+  <si>
+    <t>Un metamorfismo de esquisto de bajo grado. Presenta una superficie similar a una lámina y de color opaco.</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,4 +4014,1855 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
+  <dimension ref="A1:D201"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>430</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>431</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>432</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>433</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>434</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>361</v>
+      </c>
+      <c r="B43" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>312</v>
+      </c>
+      <c r="B46" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>368</v>
+      </c>
+      <c r="B47" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>370</v>
+      </c>
+      <c r="B48" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B49" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>397</v>
+      </c>
+      <c r="B65" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>365</v>
+      </c>
+      <c r="B67" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>367</v>
+      </c>
+      <c r="B68" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B70" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>362</v>
+      </c>
+      <c r="B72" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>364</v>
+      </c>
+      <c r="B73" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>215</v>
+      </c>
+      <c r="B76" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>216</v>
+      </c>
+      <c r="B77" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>374</v>
+      </c>
+      <c r="B81" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>376</v>
+      </c>
+      <c r="B82" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>377</v>
+      </c>
+      <c r="B83" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>223</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>224</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>225</v>
+      </c>
+      <c r="B86" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>382</v>
+      </c>
+      <c r="B87" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>230</v>
+      </c>
+      <c r="B89" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>235</v>
+      </c>
+      <c r="B90" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>237</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>238</v>
+      </c>
+      <c r="B92" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>239</v>
+      </c>
+      <c r="B93" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>241</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>247</v>
+      </c>
+      <c r="B96" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>384</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>250</v>
+      </c>
+      <c r="B99" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>251</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>252</v>
+      </c>
+      <c r="B101" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>261</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>263</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>264</v>
+      </c>
+      <c r="B106" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>265</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>268</v>
+      </c>
+      <c r="B108" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>269</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>388</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>390</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>270</v>
+      </c>
+      <c r="B113" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>271</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>272</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>303</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>305</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>307</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>277</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>283</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>279</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>281</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>205</v>
+      </c>
+      <c r="B125" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>285</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>302</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>287</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>291</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>221</v>
+      </c>
+      <c r="B131" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>394</v>
+      </c>
+      <c r="B134" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>212</v>
+      </c>
+      <c r="B135" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>208</v>
+      </c>
+      <c r="B136" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>210</v>
+      </c>
+      <c r="B137" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" t="s">
+        <v>537</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>539</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>14</v>
+      </c>
+      <c r="B141" t="s">
+        <v>540</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>108</v>
+      </c>
+      <c r="B142" t="s">
+        <v>541</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>110</v>
+      </c>
+      <c r="B143" t="s">
+        <v>542</v>
+      </c>
+      <c r="C143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>111</v>
+      </c>
+      <c r="B144" t="s">
+        <v>543</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>113</v>
+      </c>
+      <c r="B145" t="s">
+        <v>544</v>
+      </c>
+      <c r="C145">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>114</v>
+      </c>
+      <c r="B146" t="s">
+        <v>545</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>116</v>
+      </c>
+      <c r="B147" t="s">
+        <v>546</v>
+      </c>
+      <c r="C147">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>117</v>
+      </c>
+      <c r="B148" t="s">
+        <v>547</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>119</v>
+      </c>
+      <c r="B149" t="s">
+        <v>548</v>
+      </c>
+      <c r="C149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>74</v>
+      </c>
+      <c r="B150" t="s">
+        <v>549</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>75</v>
+      </c>
+      <c r="B151" t="s">
+        <v>550</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152" t="s">
+        <v>551</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>77</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C153">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" t="s">
+        <v>553</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" t="s">
+        <v>554</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156" t="s">
+        <v>555</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>20</v>
+      </c>
+      <c r="B157" t="s">
+        <v>556</v>
+      </c>
+      <c r="C157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>21</v>
+      </c>
+      <c r="B158" t="s">
+        <v>557</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" t="s">
+        <v>558</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>24</v>
+      </c>
+      <c r="B160" t="s">
+        <v>559</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" t="s">
+        <v>560</v>
+      </c>
+      <c r="C161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>33</v>
+      </c>
+      <c r="B162" t="s">
+        <v>561</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>35</v>
+      </c>
+      <c r="B163" t="s">
+        <v>562</v>
+      </c>
+      <c r="C163">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>36</v>
+      </c>
+      <c r="B164" t="s">
+        <v>563</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>38</v>
+      </c>
+      <c r="B165" t="s">
+        <v>564</v>
+      </c>
+      <c r="C165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>40</v>
+      </c>
+      <c r="B166" t="s">
+        <v>565</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>41</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>42</v>
+      </c>
+      <c r="B168" t="s">
+        <v>567</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>44</v>
+      </c>
+      <c r="B169" t="s">
+        <v>568</v>
+      </c>
+      <c r="C169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>78</v>
+      </c>
+      <c r="B170" t="s">
+        <v>569</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>80</v>
+      </c>
+      <c r="B171" t="s">
+        <v>570</v>
+      </c>
+      <c r="C171">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>45</v>
+      </c>
+      <c r="B172" t="s">
+        <v>571</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>47</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="C173">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>48</v>
+      </c>
+      <c r="B174" t="s">
+        <v>573</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>50</v>
+      </c>
+      <c r="B175" t="s">
+        <v>574</v>
+      </c>
+      <c r="C175">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>51</v>
+      </c>
+      <c r="B176" t="s">
+        <v>575</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>53</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C177">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>54</v>
+      </c>
+      <c r="B178" t="s">
+        <v>577</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>56</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C179">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>57</v>
+      </c>
+      <c r="B180" t="s">
+        <v>579</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>59</v>
+      </c>
+      <c r="B181" t="s">
+        <v>580</v>
+      </c>
+      <c r="C181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>60</v>
+      </c>
+      <c r="B182" t="s">
+        <v>581</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>62</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C183">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>81</v>
+      </c>
+      <c r="B184" t="s">
+        <v>583</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>83</v>
+      </c>
+      <c r="B185" t="s">
+        <v>584</v>
+      </c>
+      <c r="C185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>84</v>
+      </c>
+      <c r="B186" t="s">
+        <v>585</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>86</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="C187">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>87</v>
+      </c>
+      <c r="B188" t="s">
+        <v>587</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>89</v>
+      </c>
+      <c r="B189" t="s">
+        <v>588</v>
+      </c>
+      <c r="C189">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>90</v>
+      </c>
+      <c r="B190" t="s">
+        <v>589</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>92</v>
+      </c>
+      <c r="B191" t="s">
+        <v>590</v>
+      </c>
+      <c r="C191">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>93</v>
+      </c>
+      <c r="B192" t="s">
+        <v>591</v>
+      </c>
+      <c r="C192">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>95</v>
+      </c>
+      <c r="B193" t="s">
+        <v>592</v>
+      </c>
+      <c r="C193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>96</v>
+      </c>
+      <c r="B194" t="s">
+        <v>593</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>98</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C195">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>99</v>
+      </c>
+      <c r="B196" t="s">
+        <v>595</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>101</v>
+      </c>
+      <c r="B197" t="s">
+        <v>596</v>
+      </c>
+      <c r="C197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>102</v>
+      </c>
+      <c r="B198" t="s">
+        <v>575</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>104</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="C199">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>105</v>
+      </c>
+      <c r="B200" t="s">
+        <v>598</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>107</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C201">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some more UI adjustments, proper userdata usage for mockup version, added continue button at start, new build.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DCACA6-DCC4-495D-9841-4602632A6BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C703220F-8286-4F98-B55B-D730643AB547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -2168,1858 +2168,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>401</v>
-      </c>
-      <c r="B18" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B20" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>245</v>
-      </c>
-      <c r="B26" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>177</v>
-      </c>
-      <c r="B30" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>296</v>
-      </c>
-      <c r="B34" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>297</v>
-      </c>
-      <c r="B35" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>298</v>
-      </c>
-      <c r="B36" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>294</v>
-      </c>
-      <c r="B39" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>158</v>
-      </c>
-      <c r="B41" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>361</v>
-      </c>
-      <c r="B43" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>164</v>
-      </c>
-      <c r="B44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>312</v>
-      </c>
-      <c r="B46" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>368</v>
-      </c>
-      <c r="B47" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>370</v>
-      </c>
-      <c r="B48" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>372</v>
-      </c>
-      <c r="B49" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>172</v>
-      </c>
-      <c r="B50" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>185</v>
-      </c>
-      <c r="B58" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>188</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B60" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>190</v>
-      </c>
-      <c r="B61" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>191</v>
-      </c>
-      <c r="B62" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>192</v>
-      </c>
-      <c r="B63" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>196</v>
-      </c>
-      <c r="B64" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>397</v>
-      </c>
-      <c r="B65" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>198</v>
-      </c>
-      <c r="B66" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>365</v>
-      </c>
-      <c r="B67" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>367</v>
-      </c>
-      <c r="B68" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>399</v>
-      </c>
-      <c r="B69" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>200</v>
-      </c>
-      <c r="B70" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>201</v>
-      </c>
-      <c r="B71" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>362</v>
-      </c>
-      <c r="B72" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>364</v>
-      </c>
-      <c r="B73" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>213</v>
-      </c>
-      <c r="B74" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>215</v>
-      </c>
-      <c r="B76" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>216</v>
-      </c>
-      <c r="B77" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>217</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>218</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>219</v>
-      </c>
-      <c r="B80" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>374</v>
-      </c>
-      <c r="B81" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>376</v>
-      </c>
-      <c r="B82" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>377</v>
-      </c>
-      <c r="B83" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>223</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>224</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>225</v>
-      </c>
-      <c r="B86" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>382</v>
-      </c>
-      <c r="B87" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>228</v>
-      </c>
-      <c r="B88" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>230</v>
-      </c>
-      <c r="B89" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>235</v>
-      </c>
-      <c r="B90" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>237</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>238</v>
-      </c>
-      <c r="B92" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>239</v>
-      </c>
-      <c r="B93" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>240</v>
-      </c>
-      <c r="B94" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>241</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>247</v>
-      </c>
-      <c r="B96" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>248</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>384</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>250</v>
-      </c>
-      <c r="B99" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>251</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>252</v>
-      </c>
-      <c r="B101" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>259</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>260</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>261</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>263</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>264</v>
-      </c>
-      <c r="B106" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>265</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>268</v>
-      </c>
-      <c r="B108" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>269</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>388</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>390</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>392</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>270</v>
-      </c>
-      <c r="B113" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>271</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>272</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>303</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>305</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>307</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>309</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C119">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>277</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>283</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>279</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>281</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>203</v>
-      </c>
-      <c r="B124" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>205</v>
-      </c>
-      <c r="B125" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>285</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>302</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>287</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>291</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>292</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>221</v>
-      </c>
-      <c r="B131" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>253</v>
-      </c>
-      <c r="B132" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>254</v>
-      </c>
-      <c r="B133" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>394</v>
-      </c>
-      <c r="B134" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>212</v>
-      </c>
-      <c r="B135" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>208</v>
-      </c>
-      <c r="B136" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>210</v>
-      </c>
-      <c r="B137" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>10</v>
-      </c>
-      <c r="B138" t="s">
-        <v>11</v>
-      </c>
-      <c r="C138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>12</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C139">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>9</v>
-      </c>
-      <c r="B140" t="s">
-        <v>13</v>
-      </c>
-      <c r="C140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>14</v>
-      </c>
-      <c r="B141" t="s">
-        <v>326</v>
-      </c>
-      <c r="C141">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>108</v>
-      </c>
-      <c r="B142" t="s">
-        <v>109</v>
-      </c>
-      <c r="C142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>110</v>
-      </c>
-      <c r="B143" t="s">
-        <v>327</v>
-      </c>
-      <c r="C143">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>111</v>
-      </c>
-      <c r="B144" t="s">
-        <v>112</v>
-      </c>
-      <c r="C144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>113</v>
-      </c>
-      <c r="B145" t="s">
-        <v>328</v>
-      </c>
-      <c r="C145">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>114</v>
-      </c>
-      <c r="B146" t="s">
-        <v>115</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>116</v>
-      </c>
-      <c r="B147" t="s">
-        <v>329</v>
-      </c>
-      <c r="C147">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>117</v>
-      </c>
-      <c r="B148" t="s">
-        <v>118</v>
-      </c>
-      <c r="C148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>119</v>
-      </c>
-      <c r="B149" t="s">
-        <v>330</v>
-      </c>
-      <c r="C149">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>74</v>
-      </c>
-      <c r="B150" t="s">
-        <v>331</v>
-      </c>
-      <c r="C150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>75</v>
-      </c>
-      <c r="B151" t="s">
-        <v>332</v>
-      </c>
-      <c r="C151">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>76</v>
-      </c>
-      <c r="B152" t="s">
-        <v>318</v>
-      </c>
-      <c r="C152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>77</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C153">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>15</v>
-      </c>
-      <c r="B154" t="s">
-        <v>16</v>
-      </c>
-      <c r="C154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>17</v>
-      </c>
-      <c r="B155" t="s">
-        <v>334</v>
-      </c>
-      <c r="C155">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>18</v>
-      </c>
-      <c r="B156" t="s">
-        <v>19</v>
-      </c>
-      <c r="C156">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>20</v>
-      </c>
-      <c r="B157" t="s">
-        <v>319</v>
-      </c>
-      <c r="C157">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>21</v>
-      </c>
-      <c r="B158" t="s">
-        <v>22</v>
-      </c>
-      <c r="C158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>23</v>
-      </c>
-      <c r="B159" t="s">
-        <v>335</v>
-      </c>
-      <c r="C159">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>24</v>
-      </c>
-      <c r="B160" t="s">
-        <v>25</v>
-      </c>
-      <c r="C160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>26</v>
-      </c>
-      <c r="B161" t="s">
-        <v>323</v>
-      </c>
-      <c r="C161">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>33</v>
-      </c>
-      <c r="B162" t="s">
-        <v>34</v>
-      </c>
-      <c r="C162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>35</v>
-      </c>
-      <c r="B163" t="s">
-        <v>336</v>
-      </c>
-      <c r="C163">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>36</v>
-      </c>
-      <c r="B164" t="s">
-        <v>37</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>38</v>
-      </c>
-      <c r="B165" t="s">
-        <v>337</v>
-      </c>
-      <c r="C165">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>40</v>
-      </c>
-      <c r="B166" t="s">
-        <v>39</v>
-      </c>
-      <c r="C166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>41</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="C167">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>42</v>
-      </c>
-      <c r="B168" t="s">
-        <v>43</v>
-      </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>44</v>
-      </c>
-      <c r="B169" t="s">
-        <v>359</v>
-      </c>
-      <c r="C169">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>78</v>
-      </c>
-      <c r="B170" t="s">
-        <v>79</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>80</v>
-      </c>
-      <c r="B171" t="s">
-        <v>339</v>
-      </c>
-      <c r="C171">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>45</v>
-      </c>
-      <c r="B172" t="s">
-        <v>46</v>
-      </c>
-      <c r="C172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>47</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="C173">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>48</v>
-      </c>
-      <c r="B174" t="s">
-        <v>49</v>
-      </c>
-      <c r="C174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>50</v>
-      </c>
-      <c r="B175" t="s">
-        <v>320</v>
-      </c>
-      <c r="C175">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>51</v>
-      </c>
-      <c r="B176" t="s">
-        <v>52</v>
-      </c>
-      <c r="C176">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>53</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="C177">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>54</v>
-      </c>
-      <c r="B178" t="s">
-        <v>55</v>
-      </c>
-      <c r="C178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>56</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="C179">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>57</v>
-      </c>
-      <c r="B180" t="s">
-        <v>58</v>
-      </c>
-      <c r="C180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>59</v>
-      </c>
-      <c r="B181" t="s">
-        <v>343</v>
-      </c>
-      <c r="C181">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>60</v>
-      </c>
-      <c r="B182" t="s">
-        <v>61</v>
-      </c>
-      <c r="C182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>62</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="C183">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>81</v>
-      </c>
-      <c r="B184" t="s">
-        <v>82</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>83</v>
-      </c>
-      <c r="B185" t="s">
-        <v>345</v>
-      </c>
-      <c r="C185">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>84</v>
-      </c>
-      <c r="B186" t="s">
-        <v>85</v>
-      </c>
-      <c r="C186">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>86</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C187">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>87</v>
-      </c>
-      <c r="B188" t="s">
-        <v>88</v>
-      </c>
-      <c r="C188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>89</v>
-      </c>
-      <c r="B189" t="s">
-        <v>322</v>
-      </c>
-      <c r="C189">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>90</v>
-      </c>
-      <c r="B190" t="s">
-        <v>91</v>
-      </c>
-      <c r="C190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>92</v>
-      </c>
-      <c r="B191" t="s">
-        <v>321</v>
-      </c>
-      <c r="C191">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>93</v>
-      </c>
-      <c r="B192" t="s">
-        <v>94</v>
-      </c>
-      <c r="C192">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>95</v>
-      </c>
-      <c r="B193" t="s">
-        <v>347</v>
-      </c>
-      <c r="C193">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>96</v>
-      </c>
-      <c r="B194" t="s">
-        <v>97</v>
-      </c>
-      <c r="C194">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>98</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C195">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>99</v>
-      </c>
-      <c r="B196" t="s">
-        <v>100</v>
-      </c>
-      <c r="C196">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>101</v>
-      </c>
-      <c r="B197" t="s">
-        <v>324</v>
-      </c>
-      <c r="C197">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>102</v>
-      </c>
-      <c r="B198" t="s">
-        <v>103</v>
-      </c>
-      <c r="C198">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>104</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="C199">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>105</v>
-      </c>
-      <c r="B200" t="s">
-        <v>106</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>107</v>
-      </c>
-      <c r="B201" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C201">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
-  <dimension ref="A1:D201"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -4051,6 +2199,1858 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>296</v>
+      </c>
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>361</v>
+      </c>
+      <c r="B43" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>312</v>
+      </c>
+      <c r="B46" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>368</v>
+      </c>
+      <c r="B47" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>370</v>
+      </c>
+      <c r="B48" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>372</v>
+      </c>
+      <c r="B49" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B61" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>191</v>
+      </c>
+      <c r="B62" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>192</v>
+      </c>
+      <c r="B63" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>196</v>
+      </c>
+      <c r="B64" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>397</v>
+      </c>
+      <c r="B65" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>365</v>
+      </c>
+      <c r="B67" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>367</v>
+      </c>
+      <c r="B68" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>200</v>
+      </c>
+      <c r="B70" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>362</v>
+      </c>
+      <c r="B72" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>364</v>
+      </c>
+      <c r="B73" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>214</v>
+      </c>
+      <c r="B75" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>215</v>
+      </c>
+      <c r="B76" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>216</v>
+      </c>
+      <c r="B77" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>217</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>218</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>374</v>
+      </c>
+      <c r="B81" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>376</v>
+      </c>
+      <c r="B82" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>377</v>
+      </c>
+      <c r="B83" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>223</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>224</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>225</v>
+      </c>
+      <c r="B86" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>382</v>
+      </c>
+      <c r="B87" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>230</v>
+      </c>
+      <c r="B89" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>235</v>
+      </c>
+      <c r="B90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>237</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>238</v>
+      </c>
+      <c r="B92" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>239</v>
+      </c>
+      <c r="B93" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>240</v>
+      </c>
+      <c r="B94" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>241</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>247</v>
+      </c>
+      <c r="B96" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>248</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>384</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>250</v>
+      </c>
+      <c r="B99" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>251</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>252</v>
+      </c>
+      <c r="B101" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>261</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>263</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>264</v>
+      </c>
+      <c r="B106" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>265</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>268</v>
+      </c>
+      <c r="B108" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>269</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>388</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>390</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>270</v>
+      </c>
+      <c r="B113" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>271</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>272</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>303</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>305</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>307</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>309</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>277</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>283</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>279</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>281</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>205</v>
+      </c>
+      <c r="B125" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>285</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>302</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>287</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>291</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>221</v>
+      </c>
+      <c r="B131" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>394</v>
+      </c>
+      <c r="B134" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>212</v>
+      </c>
+      <c r="B135" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>208</v>
+      </c>
+      <c r="B136" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>210</v>
+      </c>
+      <c r="B137" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>9</v>
+      </c>
+      <c r="B140" t="s">
+        <v>13</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>14</v>
+      </c>
+      <c r="B141" t="s">
+        <v>326</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>108</v>
+      </c>
+      <c r="B142" t="s">
+        <v>109</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>110</v>
+      </c>
+      <c r="B143" t="s">
+        <v>327</v>
+      </c>
+      <c r="C143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>111</v>
+      </c>
+      <c r="B144" t="s">
+        <v>112</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>113</v>
+      </c>
+      <c r="B145" t="s">
+        <v>328</v>
+      </c>
+      <c r="C145">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>114</v>
+      </c>
+      <c r="B146" t="s">
+        <v>115</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>116</v>
+      </c>
+      <c r="B147" t="s">
+        <v>329</v>
+      </c>
+      <c r="C147">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>117</v>
+      </c>
+      <c r="B148" t="s">
+        <v>118</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>119</v>
+      </c>
+      <c r="B149" t="s">
+        <v>330</v>
+      </c>
+      <c r="C149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>74</v>
+      </c>
+      <c r="B150" t="s">
+        <v>331</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>75</v>
+      </c>
+      <c r="B151" t="s">
+        <v>332</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>76</v>
+      </c>
+      <c r="B152" t="s">
+        <v>318</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>77</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C153">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>15</v>
+      </c>
+      <c r="B154" t="s">
+        <v>16</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" t="s">
+        <v>334</v>
+      </c>
+      <c r="C155">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>18</v>
+      </c>
+      <c r="B156" t="s">
+        <v>19</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>20</v>
+      </c>
+      <c r="B157" t="s">
+        <v>319</v>
+      </c>
+      <c r="C157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>21</v>
+      </c>
+      <c r="B158" t="s">
+        <v>22</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" t="s">
+        <v>335</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>24</v>
+      </c>
+      <c r="B160" t="s">
+        <v>25</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" t="s">
+        <v>323</v>
+      </c>
+      <c r="C161">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>33</v>
+      </c>
+      <c r="B162" t="s">
+        <v>34</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>35</v>
+      </c>
+      <c r="B163" t="s">
+        <v>336</v>
+      </c>
+      <c r="C163">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>36</v>
+      </c>
+      <c r="B164" t="s">
+        <v>37</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>38</v>
+      </c>
+      <c r="B165" t="s">
+        <v>337</v>
+      </c>
+      <c r="C165">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>40</v>
+      </c>
+      <c r="B166" t="s">
+        <v>39</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>41</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C167">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>42</v>
+      </c>
+      <c r="B168" t="s">
+        <v>43</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>44</v>
+      </c>
+      <c r="B169" t="s">
+        <v>359</v>
+      </c>
+      <c r="C169">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>78</v>
+      </c>
+      <c r="B170" t="s">
+        <v>79</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>80</v>
+      </c>
+      <c r="B171" t="s">
+        <v>339</v>
+      </c>
+      <c r="C171">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>45</v>
+      </c>
+      <c r="B172" t="s">
+        <v>46</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>47</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C173">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>48</v>
+      </c>
+      <c r="B174" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>50</v>
+      </c>
+      <c r="B175" t="s">
+        <v>320</v>
+      </c>
+      <c r="C175">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>51</v>
+      </c>
+      <c r="B176" t="s">
+        <v>52</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>53</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C177">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>54</v>
+      </c>
+      <c r="B178" t="s">
+        <v>55</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>56</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C179">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>57</v>
+      </c>
+      <c r="B180" t="s">
+        <v>58</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>59</v>
+      </c>
+      <c r="B181" t="s">
+        <v>343</v>
+      </c>
+      <c r="C181">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>60</v>
+      </c>
+      <c r="B182" t="s">
+        <v>61</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>62</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C183">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>81</v>
+      </c>
+      <c r="B184" t="s">
+        <v>82</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>83</v>
+      </c>
+      <c r="B185" t="s">
+        <v>345</v>
+      </c>
+      <c r="C185">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>84</v>
+      </c>
+      <c r="B186" t="s">
+        <v>85</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>86</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C187">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>87</v>
+      </c>
+      <c r="B188" t="s">
+        <v>88</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>89</v>
+      </c>
+      <c r="B189" t="s">
+        <v>322</v>
+      </c>
+      <c r="C189">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>90</v>
+      </c>
+      <c r="B190" t="s">
+        <v>91</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>92</v>
+      </c>
+      <c r="B191" t="s">
+        <v>321</v>
+      </c>
+      <c r="C191">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>93</v>
+      </c>
+      <c r="B192" t="s">
+        <v>94</v>
+      </c>
+      <c r="C192">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>95</v>
+      </c>
+      <c r="B193" t="s">
+        <v>347</v>
+      </c>
+      <c r="C193">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>96</v>
+      </c>
+      <c r="B194" t="s">
+        <v>97</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>98</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C195">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>99</v>
+      </c>
+      <c r="B196" t="s">
+        <v>100</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>101</v>
+      </c>
+      <c r="B197" t="s">
+        <v>324</v>
+      </c>
+      <c r="C197">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>102</v>
+      </c>
+      <c r="B198" t="s">
+        <v>103</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>104</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C199">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>105</v>
+      </c>
+      <c r="B200" t="s">
+        <v>106</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>107</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C201">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
+  <dimension ref="A1:D201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>404</v>
       </c>
       <c r="C2">

</xml_diff>

<commit_message>
added virtual control config, ensure virtual control only shows when player is active.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C703220F-8286-4F98-B55B-D730643AB547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EF2F3-87AB-46D3-84A1-D0A95FBDC748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7875" yWindow="3810" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="610">
   <si>
     <t>Key</t>
   </si>
@@ -1821,6 +1821,36 @@
   </si>
   <si>
     <t>Un metamorfismo de esquisto de bajo grado. Presenta una superficie similar a una lámina y de color opaco.</t>
+  </si>
+  <si>
+    <t>inputConfigTitle</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>inputConfigKeyboard</t>
+  </si>
+  <si>
+    <t>inputConfigTabletRight</t>
+  </si>
+  <si>
+    <t>inputConfigTabletLeft</t>
+  </si>
+  <si>
+    <t>inputConfigTablet</t>
+  </si>
+  <si>
+    <t>Right-Handed</t>
+  </si>
+  <si>
+    <t>Left-Handed</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>Touch Screen</t>
   </si>
 </sst>
 </file>
@@ -2166,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B203" sqref="B203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,6 +4040,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>600</v>
+      </c>
+      <c r="B202" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>602</v>
+      </c>
+      <c r="B203" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>605</v>
+      </c>
+      <c r="B204" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>603</v>
+      </c>
+      <c r="B205" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>604</v>
+      </c>
+      <c r="B206" t="s">
+        <v>607</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4018,10 +4088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,6 +5932,31 @@
         <v>5</v>
       </c>
     </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed "enter" prompt in hub scene based on input type
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EF2F3-87AB-46D3-84A1-D0A95FBDC748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA71B65-C4B8-4A70-A2E6-671936944B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7875" yWindow="3810" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="614">
   <si>
     <t>Key</t>
   </si>
@@ -1851,6 +1851,18 @@
   </si>
   <si>
     <t>Touch Screen</t>
+  </si>
+  <si>
+    <t>press_to_enter</t>
+  </si>
+  <si>
+    <t>Press to Enter</t>
+  </si>
+  <si>
+    <t>press_to_jump</t>
+  </si>
+  <si>
+    <t>Press to Jump</t>
   </si>
 </sst>
 </file>
@@ -2196,10 +2208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B203" sqref="B203"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4080,6 +4092,22 @@
         <v>607</v>
       </c>
     </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>610</v>
+      </c>
+      <c r="B207" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>612</v>
+      </c>
+      <c r="B208" t="s">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4088,10 +4116,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202"/>
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5957,6 +5985,16 @@
         <v>604</v>
       </c>
     </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>612</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
some tweaks to pop-ups
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA71B65-C4B8-4A70-A2E6-671936944B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028B1E6B-6490-4CC6-8C4F-F369A7578EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7875" yWindow="3810" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="616">
   <si>
     <t>Key</t>
   </si>
@@ -1863,6 +1863,12 @@
   </si>
   <si>
     <t>Press to Jump</t>
+  </si>
+  <si>
+    <t>press_to_move</t>
+  </si>
+  <si>
+    <t>Use this to move Left or Right</t>
   </si>
 </sst>
 </file>
@@ -2208,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A208" sqref="A208"/>
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4108,6 +4114,14 @@
         <v>613</v>
       </c>
     </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>614</v>
+      </c>
+      <c r="B209" t="s">
+        <v>615</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4116,10 +4130,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
-  <dimension ref="A1:D208"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
     <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5995,6 +6009,11 @@
         <v>612</v>
       </c>
     </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new build, update language from last submit
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028B1E6B-6490-4CC6-8C4F-F369A7578EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACD63F4-00E2-4603-A786-AB3B5A8836E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="3810" windowWidth="22875" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="5040" windowWidth="26865" windowHeight="13815" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="624">
   <si>
     <t>Key</t>
   </si>
@@ -1869,6 +1869,30 @@
   </si>
   <si>
     <t>Use this to move Left or Right</t>
+  </si>
+  <si>
+    <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>Teclado</t>
+  </si>
+  <si>
+    <t>Pantalla táctil</t>
+  </si>
+  <si>
+    <t>Mano derecha</t>
+  </si>
+  <si>
+    <t>Mano izquierda</t>
+  </si>
+  <si>
+    <t>Pulsa para entrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulsa para saltar </t>
+  </si>
+  <si>
+    <t>Pulsa para moverte a la derecha o izquierda</t>
   </si>
 </sst>
 </file>
@@ -2216,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,8 +4156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1BD0E9-8E0A-4A0C-A962-0EED0A0F71DB}">
   <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="A207" sqref="A207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5978,40 +6002,64 @@
       <c r="A202" t="s">
         <v>600</v>
       </c>
+      <c r="B202" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>602</v>
       </c>
+      <c r="B203" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>605</v>
       </c>
+      <c r="B204" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>603</v>
       </c>
+      <c r="B205" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>604</v>
       </c>
+      <c r="B206" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>610</v>
       </c>
+      <c r="B207" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>614</v>
+      </c>
+      <c r="B209" t="s">
+        <v>623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>